<commit_message>
final antes da modificacao e new branch
</commit_message>
<xml_diff>
--- a/layers_dta.xlsx
+++ b/layers_dta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\python\layers performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B4E9E2-7BD7-4010-90CC-CACADE08B22F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1841202C-B6F5-4396-9D76-3D3C9800BE9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2569" uniqueCount="541">
   <si>
     <r>
       <rPr>
@@ -36561,10 +36561,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E3787F-904D-4FED-BBDE-8BED3DDF4D86}">
-  <dimension ref="A1:S84"/>
+  <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -36653,6 +36653,49 @@
       <c r="C2" t="s">
         <v>434</v>
       </c>
+      <c r="D2">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>89</v>
+      </c>
+      <c r="F2">
+        <f>E2</f>
+        <v>89</v>
+      </c>
+      <c r="G2">
+        <f>R2*(1+I2/100)</f>
+        <v>1.002</v>
+      </c>
+      <c r="H2">
+        <f>G2</f>
+        <v>1.002</v>
+      </c>
+      <c r="I2">
+        <f>100-S2</f>
+        <v>0.20000000000000284</v>
+      </c>
+      <c r="M2">
+        <v>46.1</v>
+      </c>
+      <c r="N2" s="15">
+        <f t="shared" ref="N2:N65" si="0">(F2-E2)/2+E2</f>
+        <v>89</v>
+      </c>
+      <c r="O2" s="15">
+        <f t="shared" ref="O2:O65" si="1">N2*7</f>
+        <v>623</v>
+      </c>
+      <c r="P2" s="15" t="e">
+        <f>#REF!+O2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>99.8</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
@@ -36665,44 +36708,44 @@
         <v>434</v>
       </c>
       <c r="D3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="F3">
-        <f>E3</f>
-        <v>89</v>
+        <f t="shared" ref="F3:F66" si="2">E3</f>
+        <v>97</v>
       </c>
       <c r="G3">
-        <f>R3*(1+I3/100)</f>
-        <v>1.002</v>
+        <f t="shared" ref="G3:G66" si="3">R3*(1+I3/100)</f>
+        <v>4.008</v>
       </c>
       <c r="H3">
-        <f>G3</f>
-        <v>1.002</v>
+        <f t="shared" ref="H3:H66" si="4">G3</f>
+        <v>4.008</v>
       </c>
       <c r="I3">
-        <f>100-S3</f>
+        <f t="shared" ref="I3:I66" si="5">100-S3</f>
         <v>0.20000000000000284</v>
       </c>
       <c r="M3">
-        <v>46.1</v>
+        <v>49.2</v>
       </c>
       <c r="N3" s="15">
-        <f t="shared" ref="N3:N66" si="0">(F3-E3)/2+E3</f>
-        <v>89</v>
+        <f t="shared" si="0"/>
+        <v>97</v>
       </c>
       <c r="O3" s="15">
-        <f t="shared" ref="O3:O66" si="1">N3*7</f>
-        <v>623</v>
-      </c>
-      <c r="P3" s="15">
-        <f>P2+O3</f>
-        <v>623</v>
+        <f t="shared" si="1"/>
+        <v>679</v>
+      </c>
+      <c r="P3" s="15" t="e">
+        <f t="shared" ref="P3:P66" si="6">P2+O3</f>
+        <v>#REF!</v>
       </c>
       <c r="R3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S3">
         <v>99.8</v>
@@ -36719,47 +36762,47 @@
         <v>434</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F67" si="2">E4</f>
-        <v>97</v>
+        <f t="shared" si="2"/>
+        <v>104</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G67" si="3">R4*(1+I4/100)</f>
-        <v>4.008</v>
+        <f t="shared" si="3"/>
+        <v>9.0269999999999992</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H67" si="4">G4</f>
-        <v>4.008</v>
+        <f t="shared" si="4"/>
+        <v>9.0269999999999992</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I67" si="5">100-S4</f>
-        <v>0.20000000000000284</v>
+        <f t="shared" si="5"/>
+        <v>0.29999999999999716</v>
       </c>
       <c r="M4">
-        <v>49.2</v>
+        <v>52</v>
       </c>
       <c r="N4" s="15">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="O4" s="15">
         <f t="shared" si="1"/>
-        <v>679</v>
-      </c>
-      <c r="P4" s="15">
-        <f t="shared" ref="P4:P67" si="6">P3+O4</f>
-        <v>1302</v>
+        <v>728</v>
+      </c>
+      <c r="P4" s="15" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
       </c>
       <c r="R4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S4">
-        <v>99.8</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
@@ -36773,47 +36816,47 @@
         <v>434</v>
       </c>
       <c r="D5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="G5">
         <f t="shared" si="3"/>
-        <v>9.0269999999999992</v>
+        <v>14.056000000000001</v>
       </c>
       <c r="H5">
         <f t="shared" si="4"/>
-        <v>9.0269999999999992</v>
+        <v>14.056000000000001</v>
       </c>
       <c r="I5">
         <f t="shared" si="5"/>
-        <v>0.29999999999999716</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="M5">
-        <v>52</v>
+        <v>54.2</v>
       </c>
       <c r="N5" s="15">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="O5" s="15">
         <f t="shared" si="1"/>
-        <v>728</v>
-      </c>
-      <c r="P5" s="15">
+        <v>770</v>
+      </c>
+      <c r="P5" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>2030</v>
+        <v>#REF!</v>
       </c>
       <c r="R5">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="S5">
-        <v>99.7</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
@@ -36827,47 +36870,47 @@
         <v>434</v>
       </c>
       <c r="D6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>14.056000000000001</v>
+        <v>21.104999999999997</v>
       </c>
       <c r="H6">
         <f t="shared" si="4"/>
-        <v>14.056000000000001</v>
+        <v>21.104999999999997</v>
       </c>
       <c r="I6">
         <f t="shared" si="5"/>
-        <v>0.40000000000000568</v>
+        <v>0.5</v>
       </c>
       <c r="M6">
-        <v>54.2</v>
+        <v>56</v>
       </c>
       <c r="N6" s="15">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="O6" s="15">
         <f t="shared" si="1"/>
-        <v>770</v>
-      </c>
-      <c r="P6" s="15">
+        <v>784</v>
+      </c>
+      <c r="P6" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>2800</v>
+        <v>#REF!</v>
       </c>
       <c r="R6">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="S6">
-        <v>99.6</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
@@ -36881,7 +36924,7 @@
         <v>434</v>
       </c>
       <c r="D7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <v>112</v>
@@ -36892,18 +36935,18 @@
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
-        <v>21.104999999999997</v>
+        <v>28.167999999999999</v>
       </c>
       <c r="H7">
         <f t="shared" si="4"/>
-        <v>21.104999999999997</v>
+        <v>28.167999999999999</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>0.59999999999999432</v>
       </c>
       <c r="M7">
-        <v>56</v>
+        <v>57.4</v>
       </c>
       <c r="N7" s="15">
         <f t="shared" si="0"/>
@@ -36913,15 +36956,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P7" s="15">
+      <c r="P7" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>3584</v>
+        <v>#REF!</v>
       </c>
       <c r="R7">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S7">
-        <v>99.5</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
@@ -36935,7 +36978,7 @@
         <v>434</v>
       </c>
       <c r="D8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <v>112</v>
@@ -36946,18 +36989,18 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>28.167999999999999</v>
+        <v>34.238000000000007</v>
       </c>
       <c r="H8">
         <f t="shared" si="4"/>
-        <v>28.167999999999999</v>
+        <v>34.238000000000007</v>
       </c>
       <c r="I8">
         <f t="shared" si="5"/>
-        <v>0.59999999999999432</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="M8">
-        <v>57.4</v>
+        <v>58.6</v>
       </c>
       <c r="N8" s="15">
         <f t="shared" si="0"/>
@@ -36967,15 +37010,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>4368</v>
+        <v>#REF!</v>
       </c>
       <c r="R8">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="S8">
-        <v>99.4</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
@@ -36989,7 +37032,7 @@
         <v>434</v>
       </c>
       <c r="D9">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <v>112</v>
@@ -37000,18 +37043,18 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>34.238000000000007</v>
+        <v>41.287000000000006</v>
       </c>
       <c r="H9">
         <f t="shared" si="4"/>
-        <v>34.238000000000007</v>
+        <v>41.287000000000006</v>
       </c>
       <c r="I9">
         <f t="shared" si="5"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="M9">
-        <v>58.6</v>
+        <v>59.5</v>
       </c>
       <c r="N9" s="15">
         <f t="shared" si="0"/>
@@ -37021,12 +37064,12 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>5152</v>
+        <v>#REF!</v>
       </c>
       <c r="R9">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="S9">
         <v>99.3</v>
@@ -37043,7 +37086,7 @@
         <v>434</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>112</v>
@@ -37054,18 +37097,18 @@
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>41.287000000000006</v>
+        <v>48.384</v>
       </c>
       <c r="H10">
         <f t="shared" si="4"/>
-        <v>41.287000000000006</v>
+        <v>48.384</v>
       </c>
       <c r="I10">
         <f t="shared" si="5"/>
-        <v>0.70000000000000284</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="M10">
-        <v>59.5</v>
+        <v>60.2</v>
       </c>
       <c r="N10" s="15">
         <f t="shared" si="0"/>
@@ -37075,15 +37118,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>5936</v>
+        <v>#REF!</v>
       </c>
       <c r="R10">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="S10">
-        <v>99.3</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
@@ -37097,7 +37140,7 @@
         <v>434</v>
       </c>
       <c r="D11">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11">
         <v>112</v>
@@ -37108,18 +37151,18 @@
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>48.384</v>
+        <v>54.486000000000004</v>
       </c>
       <c r="H11">
         <f t="shared" si="4"/>
-        <v>48.384</v>
+        <v>54.486000000000004</v>
       </c>
       <c r="I11">
         <f t="shared" si="5"/>
-        <v>0.79999999999999716</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="M11">
-        <v>60.2</v>
+        <v>60.8</v>
       </c>
       <c r="N11" s="15">
         <f t="shared" si="0"/>
@@ -37129,15 +37172,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>6720</v>
+        <v>#REF!</v>
       </c>
       <c r="R11">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="S11">
-        <v>99.2</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
@@ -37151,7 +37194,7 @@
         <v>434</v>
       </c>
       <c r="D12">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>112</v>
@@ -37162,18 +37205,18 @@
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>54.486000000000004</v>
+        <v>61.61</v>
       </c>
       <c r="H12">
         <f t="shared" si="4"/>
-        <v>54.486000000000004</v>
+        <v>61.61</v>
       </c>
       <c r="I12">
         <f t="shared" si="5"/>
-        <v>0.90000000000000568</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>60.8</v>
+        <v>61.2</v>
       </c>
       <c r="N12" s="15">
         <f t="shared" si="0"/>
@@ -37183,15 +37226,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>7504</v>
+        <v>#REF!</v>
       </c>
       <c r="R12">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="S12">
-        <v>99.1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
@@ -37205,7 +37248,7 @@
         <v>434</v>
       </c>
       <c r="D13">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>112</v>
@@ -37216,18 +37259,18 @@
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>61.61</v>
+        <v>68.74799999999999</v>
       </c>
       <c r="H13">
         <f t="shared" si="4"/>
-        <v>61.61</v>
+        <v>68.74799999999999</v>
       </c>
       <c r="I13">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.0999999999999943</v>
       </c>
       <c r="M13">
-        <v>61.2</v>
+        <v>61.6</v>
       </c>
       <c r="N13" s="15">
         <f t="shared" si="0"/>
@@ -37237,15 +37280,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P13" s="15">
+      <c r="P13" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>8288</v>
+        <v>#REF!</v>
       </c>
       <c r="R13">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="S13">
-        <v>99</v>
+        <v>98.9</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
@@ -37259,7 +37302,7 @@
         <v>434</v>
       </c>
       <c r="D14">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>112</v>
@@ -37270,18 +37313,18 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>68.74799999999999</v>
+        <v>74.813999999999993</v>
       </c>
       <c r="H14">
         <f t="shared" si="4"/>
-        <v>68.74799999999999</v>
+        <v>74.813999999999993</v>
       </c>
       <c r="I14">
         <f t="shared" si="5"/>
         <v>1.0999999999999943</v>
       </c>
       <c r="M14">
-        <v>61.6</v>
+        <v>61.9</v>
       </c>
       <c r="N14" s="15">
         <f t="shared" si="0"/>
@@ -37291,12 +37334,12 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P14" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>9072</v>
+        <v>#REF!</v>
       </c>
       <c r="R14">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="S14">
         <v>98.9</v>
@@ -37313,7 +37356,7 @@
         <v>434</v>
       </c>
       <c r="D15">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>112</v>
@@ -37324,18 +37367,18 @@
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>74.813999999999993</v>
+        <v>81.971999999999994</v>
       </c>
       <c r="H15">
         <f t="shared" si="4"/>
-        <v>74.813999999999993</v>
+        <v>81.971999999999994</v>
       </c>
       <c r="I15">
         <f t="shared" si="5"/>
-        <v>1.0999999999999943</v>
+        <v>1.2000000000000028</v>
       </c>
       <c r="M15">
-        <v>61.9</v>
+        <v>62.1</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" si="0"/>
@@ -37345,15 +37388,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P15" s="15">
+      <c r="P15" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>9856</v>
+        <v>#REF!</v>
       </c>
       <c r="R15">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="S15">
-        <v>98.9</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
@@ -37367,7 +37410,7 @@
         <v>434</v>
       </c>
       <c r="D16">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>112</v>
@@ -37378,18 +37421,18 @@
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>81.971999999999994</v>
+        <v>88.130999999999986</v>
       </c>
       <c r="H16">
         <f t="shared" si="4"/>
-        <v>81.971999999999994</v>
+        <v>88.130999999999986</v>
       </c>
       <c r="I16">
         <f t="shared" si="5"/>
-        <v>1.2000000000000028</v>
+        <v>1.2999999999999972</v>
       </c>
       <c r="M16">
-        <v>62.1</v>
+        <v>62.3</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="0"/>
@@ -37399,15 +37442,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>10640</v>
+        <v>#REF!</v>
       </c>
       <c r="R16">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="S16">
-        <v>98.8</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
@@ -37421,7 +37464,7 @@
         <v>434</v>
       </c>
       <c r="D17">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>112</v>
@@ -37432,18 +37475,18 @@
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>88.130999999999986</v>
+        <v>95.316000000000003</v>
       </c>
       <c r="H17">
         <f t="shared" si="4"/>
-        <v>88.130999999999986</v>
+        <v>95.316000000000003</v>
       </c>
       <c r="I17">
         <f t="shared" si="5"/>
-        <v>1.2999999999999972</v>
+        <v>1.4000000000000057</v>
       </c>
       <c r="M17">
-        <v>62.3</v>
+        <v>62.5</v>
       </c>
       <c r="N17" s="15">
         <f t="shared" si="0"/>
@@ -37453,15 +37496,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P17" s="15">
+      <c r="P17" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>11424</v>
+        <v>#REF!</v>
       </c>
       <c r="R17">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="S17">
-        <v>98.7</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
@@ -37475,7 +37518,7 @@
         <v>434</v>
       </c>
       <c r="D18">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18">
         <v>112</v>
@@ -37486,18 +37529,18 @@
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>95.316000000000003</v>
+        <v>102.51499999999999</v>
       </c>
       <c r="H18">
         <f t="shared" si="4"/>
-        <v>95.316000000000003</v>
+        <v>102.51499999999999</v>
       </c>
       <c r="I18">
         <f t="shared" si="5"/>
-        <v>1.4000000000000057</v>
+        <v>1.5</v>
       </c>
       <c r="M18">
-        <v>62.5</v>
+        <v>62.7</v>
       </c>
       <c r="N18" s="15">
         <f t="shared" si="0"/>
@@ -37507,15 +37550,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P18" s="15">
+      <c r="P18" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>12208</v>
+        <v>#REF!</v>
       </c>
       <c r="R18">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="S18">
-        <v>98.6</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
@@ -37529,7 +37572,7 @@
         <v>434</v>
       </c>
       <c r="D19">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19">
         <v>112</v>
@@ -37540,18 +37583,18 @@
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>102.51499999999999</v>
+        <v>108.712</v>
       </c>
       <c r="H19">
         <f t="shared" si="4"/>
-        <v>102.51499999999999</v>
+        <v>108.712</v>
       </c>
       <c r="I19">
         <f t="shared" si="5"/>
-        <v>1.5</v>
+        <v>1.5999999999999943</v>
       </c>
       <c r="M19">
-        <v>62.7</v>
+        <v>62.9</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" si="0"/>
@@ -37561,15 +37604,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P19" s="15">
+      <c r="P19" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>12992</v>
+        <v>#REF!</v>
       </c>
       <c r="R19">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="S19">
-        <v>98.5</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
@@ -37583,7 +37626,7 @@
         <v>434</v>
       </c>
       <c r="D20">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20">
         <v>112</v>
@@ -37594,18 +37637,18 @@
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>108.712</v>
+        <v>115.824</v>
       </c>
       <c r="H20">
         <f t="shared" si="4"/>
-        <v>108.712</v>
+        <v>115.824</v>
       </c>
       <c r="I20">
         <f t="shared" si="5"/>
         <v>1.5999999999999943</v>
       </c>
       <c r="M20">
-        <v>62.9</v>
+        <v>63.1</v>
       </c>
       <c r="N20" s="15">
         <f t="shared" si="0"/>
@@ -37615,12 +37658,12 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P20" s="15">
+      <c r="P20" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>13776</v>
+        <v>#REF!</v>
       </c>
       <c r="R20">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="S20">
         <v>98.4</v>
@@ -37637,7 +37680,7 @@
         <v>434</v>
       </c>
       <c r="D21">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>112</v>
@@ -37648,18 +37691,18 @@
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>115.824</v>
+        <v>122.04000000000002</v>
       </c>
       <c r="H21">
         <f t="shared" si="4"/>
-        <v>115.824</v>
+        <v>122.04000000000002</v>
       </c>
       <c r="I21">
         <f t="shared" si="5"/>
-        <v>1.5999999999999943</v>
+        <v>1.7000000000000028</v>
       </c>
       <c r="M21">
-        <v>63.1</v>
+        <v>63.2</v>
       </c>
       <c r="N21" s="15">
         <f t="shared" si="0"/>
@@ -37669,15 +37712,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P21" s="15">
+      <c r="P21" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>14560</v>
+        <v>#REF!</v>
       </c>
       <c r="R21">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="S21">
-        <v>98.4</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
@@ -37691,7 +37734,7 @@
         <v>434</v>
       </c>
       <c r="D22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E22">
         <v>112</v>
@@ -37702,18 +37745,18 @@
       </c>
       <c r="G22">
         <f t="shared" si="3"/>
-        <v>122.04000000000002</v>
+        <v>129.286</v>
       </c>
       <c r="H22">
         <f t="shared" si="4"/>
-        <v>122.04000000000002</v>
+        <v>129.286</v>
       </c>
       <c r="I22">
         <f t="shared" si="5"/>
-        <v>1.7000000000000028</v>
+        <v>1.7999999999999972</v>
       </c>
       <c r="M22">
-        <v>63.2</v>
+        <v>63.3</v>
       </c>
       <c r="N22" s="15">
         <f t="shared" si="0"/>
@@ -37723,15 +37766,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P22" s="15">
+      <c r="P22" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>15344</v>
+        <v>#REF!</v>
       </c>
       <c r="R22">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="S22">
-        <v>98.3</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
@@ -37745,7 +37788,7 @@
         <v>434</v>
       </c>
       <c r="D23">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>112</v>
@@ -37756,18 +37799,18 @@
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
-        <v>129.286</v>
+        <v>135.52700000000002</v>
       </c>
       <c r="H23">
         <f t="shared" si="4"/>
-        <v>129.286</v>
+        <v>135.52700000000002</v>
       </c>
       <c r="I23">
         <f t="shared" si="5"/>
-        <v>1.7999999999999972</v>
+        <v>1.9000000000000057</v>
       </c>
       <c r="M23">
-        <v>63.3</v>
+        <v>63.4</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="0"/>
@@ -37777,15 +37820,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P23" s="15">
+      <c r="P23" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>16128</v>
+        <v>#REF!</v>
       </c>
       <c r="R23">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="S23">
-        <v>98.2</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
@@ -37799,7 +37842,7 @@
         <v>434</v>
       </c>
       <c r="D24">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24">
         <v>112</v>
@@ -37810,15 +37853,15 @@
       </c>
       <c r="G24">
         <f t="shared" si="3"/>
-        <v>135.52700000000002</v>
+        <v>142.80000000000001</v>
       </c>
       <c r="H24">
         <f t="shared" si="4"/>
-        <v>135.52700000000002</v>
+        <v>142.80000000000001</v>
       </c>
       <c r="I24">
         <f t="shared" si="5"/>
-        <v>1.9000000000000057</v>
+        <v>2</v>
       </c>
       <c r="M24">
         <v>63.4</v>
@@ -37831,15 +37874,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P24" s="15">
+      <c r="P24" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>16912</v>
+        <v>#REF!</v>
       </c>
       <c r="R24">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="S24">
-        <v>98.1</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
@@ -37853,7 +37896,7 @@
         <v>434</v>
       </c>
       <c r="D25">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25">
         <v>112</v>
@@ -37864,18 +37907,18 @@
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>142.80000000000001</v>
+        <v>148.92000000000002</v>
       </c>
       <c r="H25">
         <f t="shared" si="4"/>
-        <v>142.80000000000001</v>
+        <v>148.92000000000002</v>
       </c>
       <c r="I25">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M25">
-        <v>63.4</v>
+        <v>63.5</v>
       </c>
       <c r="N25" s="15">
         <f t="shared" si="0"/>
@@ -37885,12 +37928,12 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P25" s="15">
+      <c r="P25" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>17696</v>
+        <v>#REF!</v>
       </c>
       <c r="R25">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="S25">
         <v>98</v>
@@ -37907,7 +37950,7 @@
         <v>434</v>
       </c>
       <c r="D26">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E26">
         <v>112</v>
@@ -37918,15 +37961,15 @@
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>148.92000000000002</v>
+        <v>156.21299999999999</v>
       </c>
       <c r="H26">
         <f t="shared" si="4"/>
-        <v>148.92000000000002</v>
+        <v>156.21299999999999</v>
       </c>
       <c r="I26">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>2.0999999999999943</v>
       </c>
       <c r="M26">
         <v>63.5</v>
@@ -37939,15 +37982,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P26" s="15">
+      <c r="P26" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>18480</v>
+        <v>#REF!</v>
       </c>
       <c r="R26">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="S26">
-        <v>98</v>
+        <v>97.9</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
@@ -37961,7 +38004,7 @@
         <v>434</v>
       </c>
       <c r="D27">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E27">
         <v>112</v>
@@ -37972,15 +38015,15 @@
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
-        <v>156.21299999999999</v>
+        <v>162.49799999999999</v>
       </c>
       <c r="H27">
         <f t="shared" si="4"/>
-        <v>156.21299999999999</v>
+        <v>162.49799999999999</v>
       </c>
       <c r="I27">
         <f t="shared" si="5"/>
-        <v>2.0999999999999943</v>
+        <v>2.2000000000000028</v>
       </c>
       <c r="M27">
         <v>63.5</v>
@@ -37993,15 +38036,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P27" s="15">
+      <c r="P27" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>19264</v>
+        <v>#REF!</v>
       </c>
       <c r="R27">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="S27">
-        <v>97.9</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.4">
@@ -38015,7 +38058,7 @@
         <v>434</v>
       </c>
       <c r="D28">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E28">
         <v>112</v>
@@ -38026,15 +38069,15 @@
       </c>
       <c r="G28">
         <f t="shared" si="3"/>
-        <v>162.49799999999999</v>
+        <v>168.79499999999999</v>
       </c>
       <c r="H28">
         <f t="shared" si="4"/>
-        <v>162.49799999999999</v>
+        <v>168.79499999999999</v>
       </c>
       <c r="I28">
         <f t="shared" si="5"/>
-        <v>2.2000000000000028</v>
+        <v>2.2999999999999972</v>
       </c>
       <c r="M28">
         <v>63.5</v>
@@ -38047,15 +38090,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P28" s="15">
+      <c r="P28" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>20048</v>
+        <v>#REF!</v>
       </c>
       <c r="R28">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="S28">
-        <v>97.8</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.4">
@@ -38069,7 +38112,7 @@
         <v>434</v>
       </c>
       <c r="D29">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E29">
         <v>112</v>
@@ -38080,18 +38123,18 @@
       </c>
       <c r="G29">
         <f t="shared" si="3"/>
-        <v>168.79499999999999</v>
+        <v>176.12800000000001</v>
       </c>
       <c r="H29">
         <f t="shared" si="4"/>
-        <v>168.79499999999999</v>
+        <v>176.12800000000001</v>
       </c>
       <c r="I29">
         <f t="shared" si="5"/>
-        <v>2.2999999999999972</v>
+        <v>2.4000000000000057</v>
       </c>
       <c r="M29">
-        <v>63.5</v>
+        <v>63.6</v>
       </c>
       <c r="N29" s="15">
         <f t="shared" si="0"/>
@@ -38101,15 +38144,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P29" s="15">
+      <c r="P29" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>20832</v>
+        <v>#REF!</v>
       </c>
       <c r="R29">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="S29">
-        <v>97.7</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.4">
@@ -38123,7 +38166,7 @@
         <v>434</v>
       </c>
       <c r="D30">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E30">
         <v>112</v>
@@ -38134,15 +38177,15 @@
       </c>
       <c r="G30">
         <f t="shared" si="3"/>
-        <v>176.12800000000001</v>
+        <v>182.45</v>
       </c>
       <c r="H30">
         <f t="shared" si="4"/>
-        <v>176.12800000000001</v>
+        <v>182.45</v>
       </c>
       <c r="I30">
         <f t="shared" si="5"/>
-        <v>2.4000000000000057</v>
+        <v>2.5</v>
       </c>
       <c r="M30">
         <v>63.6</v>
@@ -38155,15 +38198,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P30" s="15">
+      <c r="P30" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>21616</v>
+        <v>#REF!</v>
       </c>
       <c r="R30">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="S30">
-        <v>97.6</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.4">
@@ -38177,7 +38220,7 @@
         <v>434</v>
       </c>
       <c r="D31">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E31">
         <v>112</v>
@@ -38188,11 +38231,11 @@
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
-        <v>182.45</v>
+        <v>188.6</v>
       </c>
       <c r="H31">
         <f t="shared" si="4"/>
-        <v>182.45</v>
+        <v>188.6</v>
       </c>
       <c r="I31">
         <f t="shared" si="5"/>
@@ -38209,12 +38252,12 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P31" s="15">
+      <c r="P31" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>22400</v>
+        <v>#REF!</v>
       </c>
       <c r="R31">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="S31">
         <v>97.5</v>
@@ -38231,7 +38274,7 @@
         <v>434</v>
       </c>
       <c r="D32">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E32">
         <v>112</v>
@@ -38242,15 +38285,15 @@
       </c>
       <c r="G32">
         <f t="shared" si="3"/>
-        <v>188.6</v>
+        <v>195.96600000000001</v>
       </c>
       <c r="H32">
         <f t="shared" si="4"/>
-        <v>188.6</v>
+        <v>195.96600000000001</v>
       </c>
       <c r="I32">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>2.5999999999999943</v>
       </c>
       <c r="M32">
         <v>63.6</v>
@@ -38263,15 +38306,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P32" s="15">
+      <c r="P32" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>23184</v>
+        <v>#REF!</v>
       </c>
       <c r="R32">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="S32">
-        <v>97.5</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.4">
@@ -38285,7 +38328,7 @@
         <v>434</v>
       </c>
       <c r="D33">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E33">
         <v>112</v>
@@ -38296,15 +38339,15 @@
       </c>
       <c r="G33">
         <f t="shared" si="3"/>
-        <v>195.96600000000001</v>
+        <v>202.31900000000002</v>
       </c>
       <c r="H33">
         <f t="shared" si="4"/>
-        <v>195.96600000000001</v>
+        <v>202.31900000000002</v>
       </c>
       <c r="I33">
         <f t="shared" si="5"/>
-        <v>2.5999999999999943</v>
+        <v>2.7000000000000028</v>
       </c>
       <c r="M33">
         <v>63.6</v>
@@ -38317,15 +38360,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P33" s="15">
+      <c r="P33" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>23968</v>
+        <v>#REF!</v>
       </c>
       <c r="R33">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="S33">
-        <v>97.4</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.4">
@@ -38339,7 +38382,7 @@
         <v>434</v>
       </c>
       <c r="D34">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E34">
         <v>112</v>
@@ -38350,18 +38393,18 @@
       </c>
       <c r="G34">
         <f t="shared" si="3"/>
-        <v>202.31900000000002</v>
+        <v>208.684</v>
       </c>
       <c r="H34">
         <f t="shared" si="4"/>
-        <v>202.31900000000002</v>
+        <v>208.684</v>
       </c>
       <c r="I34">
         <f t="shared" si="5"/>
-        <v>2.7000000000000028</v>
+        <v>2.7999999999999972</v>
       </c>
       <c r="M34">
-        <v>63.6</v>
+        <v>63.7</v>
       </c>
       <c r="N34" s="15">
         <f t="shared" si="0"/>
@@ -38371,15 +38414,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P34" s="15">
+      <c r="P34" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>24752</v>
+        <v>#REF!</v>
       </c>
       <c r="R34">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="S34">
-        <v>97.3</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.4">
@@ -38393,7 +38436,7 @@
         <v>434</v>
       </c>
       <c r="D35">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E35">
         <v>112</v>
@@ -38404,15 +38447,15 @@
       </c>
       <c r="G35">
         <f t="shared" si="3"/>
-        <v>208.684</v>
+        <v>215.06100000000004</v>
       </c>
       <c r="H35">
         <f t="shared" si="4"/>
-        <v>208.684</v>
+        <v>215.06100000000004</v>
       </c>
       <c r="I35">
         <f t="shared" si="5"/>
-        <v>2.7999999999999972</v>
+        <v>2.9000000000000057</v>
       </c>
       <c r="M35">
         <v>63.7</v>
@@ -38425,15 +38468,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P35" s="15">
+      <c r="P35" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>25536</v>
+        <v>#REF!</v>
       </c>
       <c r="R35">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="S35">
-        <v>97.2</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.4">
@@ -38447,7 +38490,7 @@
         <v>434</v>
       </c>
       <c r="D36">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E36">
         <v>112</v>
@@ -38458,15 +38501,15 @@
       </c>
       <c r="G36">
         <f t="shared" si="3"/>
-        <v>215.06100000000004</v>
+        <v>222.48000000000002</v>
       </c>
       <c r="H36">
         <f t="shared" si="4"/>
-        <v>215.06100000000004</v>
+        <v>222.48000000000002</v>
       </c>
       <c r="I36">
         <f t="shared" si="5"/>
-        <v>2.9000000000000057</v>
+        <v>3</v>
       </c>
       <c r="M36">
         <v>63.7</v>
@@ -38479,15 +38522,15 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P36" s="15">
+      <c r="P36" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>26320</v>
+        <v>#REF!</v>
       </c>
       <c r="R36">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="S36">
-        <v>97.1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.4">
@@ -38501,44 +38544,44 @@
         <v>434</v>
       </c>
       <c r="D37">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E37">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G37">
         <f t="shared" si="3"/>
-        <v>222.48000000000002</v>
+        <v>228.66</v>
       </c>
       <c r="H37">
         <f t="shared" si="4"/>
-        <v>222.48000000000002</v>
+        <v>228.66</v>
       </c>
       <c r="I37">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M37">
-        <v>63.7</v>
+        <v>63.8</v>
       </c>
       <c r="N37" s="15">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O37" s="15">
         <f t="shared" si="1"/>
-        <v>784</v>
-      </c>
-      <c r="P37" s="15">
+        <v>791</v>
+      </c>
+      <c r="P37" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>27104</v>
+        <v>#REF!</v>
       </c>
       <c r="R37">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="S37">
         <v>97</v>
@@ -38555,7 +38598,7 @@
         <v>434</v>
       </c>
       <c r="D38">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E38">
         <v>113</v>
@@ -38566,15 +38609,15 @@
       </c>
       <c r="G38">
         <f t="shared" si="3"/>
-        <v>228.66</v>
+        <v>235.06799999999998</v>
       </c>
       <c r="H38">
         <f t="shared" si="4"/>
-        <v>228.66</v>
+        <v>235.06799999999998</v>
       </c>
       <c r="I38">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>3.0999999999999943</v>
       </c>
       <c r="M38">
         <v>63.8</v>
@@ -38587,15 +38630,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P38" s="15">
+      <c r="P38" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>27895</v>
+        <v>#REF!</v>
       </c>
       <c r="R38">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="S38">
-        <v>97</v>
+        <v>96.9</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.4">
@@ -38609,7 +38652,7 @@
         <v>434</v>
       </c>
       <c r="D39">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E39">
         <v>113</v>
@@ -38620,15 +38663,15 @@
       </c>
       <c r="G39">
         <f t="shared" si="3"/>
-        <v>235.06799999999998</v>
+        <v>241.488</v>
       </c>
       <c r="H39">
         <f t="shared" si="4"/>
-        <v>235.06799999999998</v>
+        <v>241.488</v>
       </c>
       <c r="I39">
         <f t="shared" si="5"/>
-        <v>3.0999999999999943</v>
+        <v>3.2000000000000028</v>
       </c>
       <c r="M39">
         <v>63.8</v>
@@ -38641,15 +38684,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P39" s="15">
+      <c r="P39" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>28686</v>
+        <v>#REF!</v>
       </c>
       <c r="R39">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="S39">
-        <v>96.9</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.4">
@@ -38663,7 +38706,7 @@
         <v>434</v>
       </c>
       <c r="D40">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E40">
         <v>113</v>
@@ -38674,15 +38717,15 @@
       </c>
       <c r="G40">
         <f t="shared" si="3"/>
-        <v>241.488</v>
+        <v>247.92</v>
       </c>
       <c r="H40">
         <f t="shared" si="4"/>
-        <v>241.488</v>
+        <v>247.92</v>
       </c>
       <c r="I40">
         <f t="shared" si="5"/>
-        <v>3.2000000000000028</v>
+        <v>3.2999999999999972</v>
       </c>
       <c r="M40">
         <v>63.8</v>
@@ -38695,15 +38738,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P40" s="15">
+      <c r="P40" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>29477</v>
+        <v>#REF!</v>
       </c>
       <c r="R40">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="S40">
-        <v>96.8</v>
+        <v>96.7</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.4">
@@ -38717,7 +38760,7 @@
         <v>434</v>
       </c>
       <c r="D41">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E41">
         <v>113</v>
@@ -38728,18 +38771,18 @@
       </c>
       <c r="G41">
         <f t="shared" si="3"/>
-        <v>247.92</v>
+        <v>254.364</v>
       </c>
       <c r="H41">
         <f t="shared" si="4"/>
-        <v>247.92</v>
+        <v>254.364</v>
       </c>
       <c r="I41">
         <f t="shared" si="5"/>
-        <v>3.2999999999999972</v>
+        <v>3.4000000000000057</v>
       </c>
       <c r="M41">
-        <v>63.8</v>
+        <v>63.9</v>
       </c>
       <c r="N41" s="15">
         <f t="shared" si="0"/>
@@ -38749,15 +38792,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P41" s="15">
+      <c r="P41" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>30268</v>
+        <v>#REF!</v>
       </c>
       <c r="R41">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="S41">
-        <v>96.7</v>
+        <v>96.6</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.4">
@@ -38771,7 +38814,7 @@
         <v>434</v>
       </c>
       <c r="D42">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E42">
         <v>113</v>
@@ -38782,11 +38825,11 @@
       </c>
       <c r="G42">
         <f t="shared" si="3"/>
-        <v>254.364</v>
+        <v>260.56799999999998</v>
       </c>
       <c r="H42">
         <f t="shared" si="4"/>
-        <v>254.364</v>
+        <v>260.56799999999998</v>
       </c>
       <c r="I42">
         <f t="shared" si="5"/>
@@ -38803,12 +38846,12 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P42" s="15">
+      <c r="P42" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>31059</v>
+        <v>#REF!</v>
       </c>
       <c r="R42">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="S42">
         <v>96.6</v>
@@ -38825,7 +38868,7 @@
         <v>434</v>
       </c>
       <c r="D43">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E43">
         <v>113</v>
@@ -38836,15 +38879,15 @@
       </c>
       <c r="G43">
         <f t="shared" si="3"/>
-        <v>260.56799999999998</v>
+        <v>267.02999999999997</v>
       </c>
       <c r="H43">
         <f t="shared" si="4"/>
-        <v>260.56799999999998</v>
+        <v>267.02999999999997</v>
       </c>
       <c r="I43">
         <f t="shared" si="5"/>
-        <v>3.4000000000000057</v>
+        <v>3.5</v>
       </c>
       <c r="M43">
         <v>63.9</v>
@@ -38857,15 +38900,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P43" s="15">
+      <c r="P43" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>31850</v>
+        <v>#REF!</v>
       </c>
       <c r="R43">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="S43">
-        <v>96.6</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.4">
@@ -38879,7 +38922,7 @@
         <v>434</v>
       </c>
       <c r="D44">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E44">
         <v>113</v>
@@ -38890,11 +38933,11 @@
       </c>
       <c r="G44">
         <f t="shared" si="3"/>
-        <v>267.02999999999997</v>
+        <v>273.23999999999995</v>
       </c>
       <c r="H44">
         <f t="shared" si="4"/>
-        <v>267.02999999999997</v>
+        <v>273.23999999999995</v>
       </c>
       <c r="I44">
         <f t="shared" si="5"/>
@@ -38911,12 +38954,12 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P44" s="15">
+      <c r="P44" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>32641</v>
+        <v>#REF!</v>
       </c>
       <c r="R44">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="S44">
         <v>96.5</v>
@@ -38933,7 +38976,7 @@
         <v>434</v>
       </c>
       <c r="D45">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E45">
         <v>113</v>
@@ -38944,18 +38987,18 @@
       </c>
       <c r="G45">
         <f t="shared" si="3"/>
-        <v>273.23999999999995</v>
+        <v>279.98999999999995</v>
       </c>
       <c r="H45">
         <f t="shared" si="4"/>
-        <v>273.23999999999995</v>
+        <v>279.98999999999995</v>
       </c>
       <c r="I45">
         <f t="shared" si="5"/>
-        <v>3.5</v>
+        <v>3.7000000000000028</v>
       </c>
       <c r="M45">
-        <v>63.9</v>
+        <v>64</v>
       </c>
       <c r="N45" s="15">
         <f t="shared" si="0"/>
@@ -38965,15 +39008,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P45" s="15">
+      <c r="P45" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>33432</v>
+        <v>#REF!</v>
       </c>
       <c r="R45">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="S45">
-        <v>96.5</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.4">
@@ -38987,7 +39030,7 @@
         <v>434</v>
       </c>
       <c r="D46">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E46">
         <v>113</v>
@@ -38998,15 +39041,15 @@
       </c>
       <c r="G46">
         <f t="shared" si="3"/>
-        <v>279.98999999999995</v>
+        <v>286.488</v>
       </c>
       <c r="H46">
         <f t="shared" si="4"/>
-        <v>279.98999999999995</v>
+        <v>286.488</v>
       </c>
       <c r="I46">
         <f t="shared" si="5"/>
-        <v>3.7000000000000028</v>
+        <v>3.7999999999999972</v>
       </c>
       <c r="M46">
         <v>64</v>
@@ -39019,15 +39062,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P46" s="15">
+      <c r="P46" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>34223</v>
+        <v>#REF!</v>
       </c>
       <c r="R46">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="S46">
-        <v>96.3</v>
+        <v>96.2</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.4">
@@ -39041,7 +39084,7 @@
         <v>434</v>
       </c>
       <c r="D47">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E47">
         <v>113</v>
@@ -39052,15 +39095,15 @@
       </c>
       <c r="G47">
         <f t="shared" si="3"/>
-        <v>286.488</v>
+        <v>291.95900000000006</v>
       </c>
       <c r="H47">
         <f t="shared" si="4"/>
-        <v>286.488</v>
+        <v>291.95900000000006</v>
       </c>
       <c r="I47">
         <f t="shared" si="5"/>
-        <v>3.7999999999999972</v>
+        <v>3.9000000000000057</v>
       </c>
       <c r="M47">
         <v>64</v>
@@ -39073,15 +39116,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P47" s="15">
+      <c r="P47" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>35014</v>
+        <v>#REF!</v>
       </c>
       <c r="R47">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="S47">
-        <v>96.2</v>
+        <v>96.1</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.4">
@@ -39095,7 +39138,7 @@
         <v>434</v>
       </c>
       <c r="D48">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E48">
         <v>113</v>
@@ -39106,11 +39149,11 @@
       </c>
       <c r="G48">
         <f t="shared" si="3"/>
-        <v>291.95900000000006</v>
+        <v>298.19300000000004</v>
       </c>
       <c r="H48">
         <f t="shared" si="4"/>
-        <v>291.95900000000006</v>
+        <v>298.19300000000004</v>
       </c>
       <c r="I48">
         <f t="shared" si="5"/>
@@ -39127,12 +39170,12 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P48" s="15">
+      <c r="P48" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>35805</v>
+        <v>#REF!</v>
       </c>
       <c r="R48">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="S48">
         <v>96.1</v>
@@ -39149,7 +39192,7 @@
         <v>434</v>
       </c>
       <c r="D49">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E49">
         <v>113</v>
@@ -39160,18 +39203,18 @@
       </c>
       <c r="G49">
         <f t="shared" si="3"/>
-        <v>298.19300000000004</v>
+        <v>304.72000000000003</v>
       </c>
       <c r="H49">
         <f t="shared" si="4"/>
-        <v>298.19300000000004</v>
+        <v>304.72000000000003</v>
       </c>
       <c r="I49">
         <f t="shared" si="5"/>
-        <v>3.9000000000000057</v>
+        <v>4</v>
       </c>
       <c r="M49">
-        <v>64</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="N49" s="15">
         <f t="shared" si="0"/>
@@ -39181,15 +39224,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P49" s="15">
+      <c r="P49" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>36596</v>
+        <v>#REF!</v>
       </c>
       <c r="R49">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="S49">
-        <v>96.1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.4">
@@ -39203,7 +39246,7 @@
         <v>434</v>
       </c>
       <c r="D50">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E50">
         <v>113</v>
@@ -39214,15 +39257,15 @@
       </c>
       <c r="G50">
         <f t="shared" si="3"/>
-        <v>304.72000000000003</v>
+        <v>311.25899999999996</v>
       </c>
       <c r="H50">
         <f t="shared" si="4"/>
-        <v>304.72000000000003</v>
+        <v>311.25899999999996</v>
       </c>
       <c r="I50">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>4.0999999999999943</v>
       </c>
       <c r="M50">
         <v>64.099999999999994</v>
@@ -39235,15 +39278,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P50" s="15">
+      <c r="P50" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>37387</v>
+        <v>#REF!</v>
       </c>
       <c r="R50">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="S50">
-        <v>96</v>
+        <v>95.9</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.4">
@@ -39257,7 +39300,7 @@
         <v>434</v>
       </c>
       <c r="D51">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E51">
         <v>113</v>
@@ -39268,15 +39311,15 @@
       </c>
       <c r="G51">
         <f t="shared" si="3"/>
-        <v>311.25899999999996</v>
+        <v>316.76800000000003</v>
       </c>
       <c r="H51">
         <f t="shared" si="4"/>
-        <v>311.25899999999996</v>
+        <v>316.76800000000003</v>
       </c>
       <c r="I51">
         <f t="shared" si="5"/>
-        <v>4.0999999999999943</v>
+        <v>4.2000000000000028</v>
       </c>
       <c r="M51">
         <v>64.099999999999994</v>
@@ -39289,15 +39332,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P51" s="15">
+      <c r="P51" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>38178</v>
+        <v>#REF!</v>
       </c>
       <c r="R51">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="S51">
-        <v>95.9</v>
+        <v>95.8</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.4">
@@ -39311,7 +39354,7 @@
         <v>434</v>
       </c>
       <c r="D52">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E52">
         <v>113</v>
@@ -39322,15 +39365,15 @@
       </c>
       <c r="G52">
         <f t="shared" si="3"/>
-        <v>316.76800000000003</v>
+        <v>323.33</v>
       </c>
       <c r="H52">
         <f t="shared" si="4"/>
-        <v>316.76800000000003</v>
+        <v>323.33</v>
       </c>
       <c r="I52">
         <f t="shared" si="5"/>
-        <v>4.2000000000000028</v>
+        <v>4.2999999999999972</v>
       </c>
       <c r="M52">
         <v>64.099999999999994</v>
@@ -39343,15 +39386,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P52" s="15">
+      <c r="P52" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>38969</v>
+        <v>#REF!</v>
       </c>
       <c r="R52">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S52">
-        <v>95.8</v>
+        <v>95.7</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.4">
@@ -39365,7 +39408,7 @@
         <v>434</v>
       </c>
       <c r="D53">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E53">
         <v>113</v>
@@ -39376,18 +39419,18 @@
       </c>
       <c r="G53">
         <f t="shared" si="3"/>
-        <v>323.33</v>
+        <v>328.54499999999996</v>
       </c>
       <c r="H53">
         <f t="shared" si="4"/>
-        <v>323.33</v>
+        <v>328.54499999999996</v>
       </c>
       <c r="I53">
         <f t="shared" si="5"/>
         <v>4.2999999999999972</v>
       </c>
       <c r="M53">
-        <v>64.099999999999994</v>
+        <v>64.2</v>
       </c>
       <c r="N53" s="15">
         <f t="shared" si="0"/>
@@ -39397,12 +39440,12 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P53" s="15">
+      <c r="P53" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>39760</v>
+        <v>#REF!</v>
       </c>
       <c r="R53">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="S53">
         <v>95.7</v>
@@ -39419,7 +39462,7 @@
         <v>434</v>
       </c>
       <c r="D54">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E54">
         <v>113</v>
@@ -39430,15 +39473,15 @@
       </c>
       <c r="G54">
         <f t="shared" si="3"/>
-        <v>328.54499999999996</v>
+        <v>335.12400000000002</v>
       </c>
       <c r="H54">
         <f t="shared" si="4"/>
-        <v>328.54499999999996</v>
+        <v>335.12400000000002</v>
       </c>
       <c r="I54">
         <f t="shared" si="5"/>
-        <v>4.2999999999999972</v>
+        <v>4.4000000000000057</v>
       </c>
       <c r="M54">
         <v>64.2</v>
@@ -39451,15 +39494,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P54" s="15">
+      <c r="P54" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>40551</v>
+        <v>#REF!</v>
       </c>
       <c r="R54">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="S54">
-        <v>95.7</v>
+        <v>95.6</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.4">
@@ -39473,7 +39516,7 @@
         <v>434</v>
       </c>
       <c r="D55">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E55">
         <v>113</v>
@@ -39484,15 +39527,15 @@
       </c>
       <c r="G55">
         <f t="shared" si="3"/>
-        <v>335.12400000000002</v>
+        <v>341.71499999999997</v>
       </c>
       <c r="H55">
         <f t="shared" si="4"/>
-        <v>335.12400000000002</v>
+        <v>341.71499999999997</v>
       </c>
       <c r="I55">
         <f t="shared" si="5"/>
-        <v>4.4000000000000057</v>
+        <v>4.5</v>
       </c>
       <c r="M55">
         <v>64.2</v>
@@ -39505,15 +39548,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P55" s="15">
+      <c r="P55" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>41342</v>
+        <v>#REF!</v>
       </c>
       <c r="R55">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="S55">
-        <v>95.6</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.4">
@@ -39527,7 +39570,7 @@
         <v>434</v>
       </c>
       <c r="D56">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E56">
         <v>113</v>
@@ -39538,15 +39581,15 @@
       </c>
       <c r="G56">
         <f t="shared" si="3"/>
-        <v>341.71499999999997</v>
+        <v>347.27199999999999</v>
       </c>
       <c r="H56">
         <f t="shared" si="4"/>
-        <v>341.71499999999997</v>
+        <v>347.27199999999999</v>
       </c>
       <c r="I56">
         <f t="shared" si="5"/>
-        <v>4.5</v>
+        <v>4.5999999999999943</v>
       </c>
       <c r="M56">
         <v>64.2</v>
@@ -39559,15 +39602,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P56" s="15">
+      <c r="P56" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>42133</v>
+        <v>#REF!</v>
       </c>
       <c r="R56">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="S56">
-        <v>95.5</v>
+        <v>95.4</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.4">
@@ -39581,7 +39624,7 @@
         <v>434</v>
       </c>
       <c r="D57">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E57">
         <v>113</v>
@@ -39592,18 +39635,18 @@
       </c>
       <c r="G57">
         <f t="shared" si="3"/>
-        <v>347.27199999999999</v>
+        <v>352.839</v>
       </c>
       <c r="H57">
         <f t="shared" si="4"/>
-        <v>347.27199999999999</v>
+        <v>352.839</v>
       </c>
       <c r="I57">
         <f t="shared" si="5"/>
-        <v>4.5999999999999943</v>
+        <v>4.7000000000000028</v>
       </c>
       <c r="M57">
-        <v>64.2</v>
+        <v>64.3</v>
       </c>
       <c r="N57" s="15">
         <f t="shared" si="0"/>
@@ -39613,15 +39656,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P57" s="15">
+      <c r="P57" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>42924</v>
+        <v>#REF!</v>
       </c>
       <c r="R57">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="S57">
-        <v>95.4</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.4">
@@ -39635,7 +39678,7 @@
         <v>434</v>
       </c>
       <c r="D58">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E58">
         <v>113</v>
@@ -39646,15 +39689,15 @@
       </c>
       <c r="G58">
         <f t="shared" si="3"/>
-        <v>352.839</v>
+        <v>359.464</v>
       </c>
       <c r="H58">
         <f t="shared" si="4"/>
-        <v>352.839</v>
+        <v>359.464</v>
       </c>
       <c r="I58">
         <f t="shared" si="5"/>
-        <v>4.7000000000000028</v>
+        <v>4.7999999999999972</v>
       </c>
       <c r="M58">
         <v>64.3</v>
@@ -39667,15 +39710,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P58" s="15">
+      <c r="P58" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>43715</v>
+        <v>#REF!</v>
       </c>
       <c r="R58">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="S58">
-        <v>95.3</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.4">
@@ -39689,7 +39732,7 @@
         <v>434</v>
       </c>
       <c r="D59">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E59">
         <v>113</v>
@@ -39700,11 +39743,11 @@
       </c>
       <c r="G59">
         <f t="shared" si="3"/>
-        <v>359.464</v>
+        <v>364.70400000000001</v>
       </c>
       <c r="H59">
         <f t="shared" si="4"/>
-        <v>359.464</v>
+        <v>364.70400000000001</v>
       </c>
       <c r="I59">
         <f t="shared" si="5"/>
@@ -39721,12 +39764,12 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P59" s="15">
+      <c r="P59" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>44506</v>
+        <v>#REF!</v>
       </c>
       <c r="R59">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="S59">
         <v>95.2</v>
@@ -39743,7 +39786,7 @@
         <v>434</v>
       </c>
       <c r="D60">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E60">
         <v>113</v>
@@ -39754,15 +39797,15 @@
       </c>
       <c r="G60">
         <f t="shared" si="3"/>
-        <v>364.70400000000001</v>
+        <v>371.34600000000006</v>
       </c>
       <c r="H60">
         <f t="shared" si="4"/>
-        <v>364.70400000000001</v>
+        <v>371.34600000000006</v>
       </c>
       <c r="I60">
         <f t="shared" si="5"/>
-        <v>4.7999999999999972</v>
+        <v>4.9000000000000057</v>
       </c>
       <c r="M60">
         <v>64.3</v>
@@ -39775,15 +39818,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P60" s="15">
+      <c r="P60" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>45297</v>
+        <v>#REF!</v>
       </c>
       <c r="R60">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="S60">
-        <v>95.2</v>
+        <v>95.1</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.4">
@@ -39797,7 +39840,7 @@
         <v>434</v>
       </c>
       <c r="D61">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E61">
         <v>113</v>
@@ -39808,18 +39851,18 @@
       </c>
       <c r="G61">
         <f t="shared" si="3"/>
-        <v>371.34600000000006</v>
+        <v>376.95</v>
       </c>
       <c r="H61">
         <f t="shared" si="4"/>
-        <v>371.34600000000006</v>
+        <v>376.95</v>
       </c>
       <c r="I61">
         <f t="shared" si="5"/>
-        <v>4.9000000000000057</v>
+        <v>5</v>
       </c>
       <c r="M61">
-        <v>64.3</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="N61" s="15">
         <f t="shared" si="0"/>
@@ -39829,15 +39872,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P61" s="15">
+      <c r="P61" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>46088</v>
+        <v>#REF!</v>
       </c>
       <c r="R61">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="S61">
-        <v>95.1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.4">
@@ -39851,7 +39894,7 @@
         <v>434</v>
       </c>
       <c r="D62">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E62">
         <v>113</v>
@@ -39862,15 +39905,15 @@
       </c>
       <c r="G62">
         <f t="shared" si="3"/>
-        <v>376.95</v>
+        <v>382.56399999999996</v>
       </c>
       <c r="H62">
         <f t="shared" si="4"/>
-        <v>376.95</v>
+        <v>382.56399999999996</v>
       </c>
       <c r="I62">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>5.0999999999999943</v>
       </c>
       <c r="M62">
         <v>64.400000000000006</v>
@@ -39883,15 +39926,15 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P62" s="15">
+      <c r="P62" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>46879</v>
+        <v>#REF!</v>
       </c>
       <c r="R62">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="S62">
-        <v>95</v>
+        <v>94.9</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.4">
@@ -39905,47 +39948,47 @@
         <v>434</v>
       </c>
       <c r="D63">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E63">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F63">
         <f t="shared" si="2"/>
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G63">
         <f t="shared" si="3"/>
-        <v>382.56399999999996</v>
+        <v>388.18800000000005</v>
       </c>
       <c r="H63">
         <f t="shared" si="4"/>
-        <v>382.56399999999996</v>
+        <v>388.18800000000005</v>
       </c>
       <c r="I63">
         <f t="shared" si="5"/>
-        <v>5.0999999999999943</v>
+        <v>5.2000000000000028</v>
       </c>
       <c r="M63">
         <v>64.400000000000006</v>
       </c>
       <c r="N63" s="15">
         <f t="shared" si="0"/>
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O63" s="15">
         <f t="shared" si="1"/>
-        <v>791</v>
-      </c>
-      <c r="P63" s="15">
+        <v>798</v>
+      </c>
+      <c r="P63" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>47670</v>
+        <v>#REF!</v>
       </c>
       <c r="R63">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="S63">
-        <v>94.9</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.4">
@@ -39959,7 +40002,7 @@
         <v>434</v>
       </c>
       <c r="D64">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E64">
         <v>114</v>
@@ -39970,11 +40013,11 @@
       </c>
       <c r="G64">
         <f t="shared" si="3"/>
-        <v>388.18800000000005</v>
+        <v>394.5</v>
       </c>
       <c r="H64">
         <f t="shared" si="4"/>
-        <v>388.18800000000005</v>
+        <v>394.5</v>
       </c>
       <c r="I64">
         <f t="shared" si="5"/>
@@ -39991,12 +40034,12 @@
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
-      <c r="P64" s="15">
+      <c r="P64" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>48468</v>
+        <v>#REF!</v>
       </c>
       <c r="R64">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="S64">
         <v>94.8</v>
@@ -40013,7 +40056,7 @@
         <v>434</v>
       </c>
       <c r="D65">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E65">
         <v>114</v>
@@ -40024,18 +40067,18 @@
       </c>
       <c r="G65">
         <f t="shared" si="3"/>
-        <v>394.5</v>
+        <v>400.14</v>
       </c>
       <c r="H65">
         <f t="shared" si="4"/>
-        <v>394.5</v>
+        <v>400.14</v>
       </c>
       <c r="I65">
         <f t="shared" si="5"/>
-        <v>5.2000000000000028</v>
+        <v>5.2999999999999972</v>
       </c>
       <c r="M65">
-        <v>64.400000000000006</v>
+        <v>64.5</v>
       </c>
       <c r="N65" s="15">
         <f t="shared" si="0"/>
@@ -40045,15 +40088,15 @@
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
-      <c r="P65" s="15">
+      <c r="P65" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>49266</v>
+        <v>#REF!</v>
       </c>
       <c r="R65">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="S65">
-        <v>94.8</v>
+        <v>94.7</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.4">
@@ -40067,7 +40110,7 @@
         <v>434</v>
       </c>
       <c r="D66">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E66">
         <v>114</v>
@@ -40078,36 +40121,36 @@
       </c>
       <c r="G66">
         <f t="shared" si="3"/>
-        <v>400.14</v>
+        <v>405.79</v>
       </c>
       <c r="H66">
         <f t="shared" si="4"/>
-        <v>400.14</v>
+        <v>405.79</v>
       </c>
       <c r="I66">
         <f t="shared" si="5"/>
-        <v>5.2999999999999972</v>
+        <v>5.4000000000000057</v>
       </c>
       <c r="M66">
         <v>64.5</v>
       </c>
       <c r="N66" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N66:N73" si="7">(F66-E66)/2+E66</f>
         <v>114</v>
       </c>
       <c r="O66" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="O66:O73" si="8">N66*7</f>
         <v>798</v>
       </c>
-      <c r="P66" s="15">
+      <c r="P66" s="15" t="e">
         <f t="shared" si="6"/>
-        <v>50064</v>
+        <v>#REF!</v>
       </c>
       <c r="R66">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="S66">
-        <v>94.7</v>
+        <v>94.6</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.4">
@@ -40121,47 +40164,47 @@
         <v>434</v>
       </c>
       <c r="D67">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E67">
         <v>114</v>
       </c>
       <c r="F67">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F67:F73" si="9">E67</f>
         <v>114</v>
       </c>
       <c r="G67">
-        <f t="shared" si="3"/>
-        <v>405.79</v>
+        <f t="shared" ref="G67:G73" si="10">R67*(1+I67/100)</f>
+        <v>411.45</v>
       </c>
       <c r="H67">
-        <f t="shared" si="4"/>
-        <v>405.79</v>
+        <f t="shared" ref="H67:H72" si="11">G67</f>
+        <v>411.45</v>
       </c>
       <c r="I67">
-        <f t="shared" si="5"/>
-        <v>5.4000000000000057</v>
+        <f t="shared" ref="I67:I73" si="12">100-S67</f>
+        <v>5.5</v>
       </c>
       <c r="M67">
         <v>64.5</v>
       </c>
       <c r="N67" s="15">
-        <f t="shared" ref="N67:N84" si="7">(F67-E67)/2+E67</f>
+        <f t="shared" si="7"/>
         <v>114</v>
       </c>
       <c r="O67" s="15">
-        <f t="shared" ref="O67:O84" si="8">N67*7</f>
+        <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P67" s="15">
-        <f t="shared" si="6"/>
-        <v>50862</v>
+      <c r="P67" s="15" t="e">
+        <f t="shared" ref="P67:P73" si="13">P66+O67</f>
+        <v>#REF!</v>
       </c>
       <c r="R67">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="S67">
-        <v>94.6</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.4">
@@ -40175,26 +40218,26 @@
         <v>434</v>
       </c>
       <c r="D68">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E68">
         <v>114</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F84" si="9">E68</f>
+        <f t="shared" si="9"/>
         <v>114</v>
       </c>
       <c r="G68">
-        <f t="shared" ref="G68:G84" si="10">R68*(1+I68/100)</f>
-        <v>411.45</v>
+        <f t="shared" si="10"/>
+        <v>417.12</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="H68:H73" si="11">G68</f>
-        <v>411.45</v>
+        <f t="shared" si="11"/>
+        <v>417.12</v>
       </c>
       <c r="I68">
-        <f t="shared" ref="I68:I84" si="12">100-S68</f>
-        <v>5.5</v>
+        <f t="shared" si="12"/>
+        <v>5.5999999999999943</v>
       </c>
       <c r="M68">
         <v>64.5</v>
@@ -40207,15 +40250,15 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P68" s="15">
-        <f t="shared" ref="P68:P84" si="13">P67+O68</f>
-        <v>51660</v>
+      <c r="P68" s="15" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="R68">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="S68">
-        <v>94.5</v>
+        <v>94.4</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.4">
@@ -40229,7 +40272,7 @@
         <v>434</v>
       </c>
       <c r="D69">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E69">
         <v>114</v>
@@ -40240,18 +40283,18 @@
       </c>
       <c r="G69">
         <f t="shared" si="10"/>
-        <v>417.12</v>
+        <v>422.79999999999995</v>
       </c>
       <c r="H69">
         <f t="shared" si="11"/>
-        <v>417.12</v>
+        <v>422.79999999999995</v>
       </c>
       <c r="I69">
         <f t="shared" si="12"/>
-        <v>5.5999999999999943</v>
+        <v>5.7000000000000028</v>
       </c>
       <c r="M69">
-        <v>64.5</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="N69" s="15">
         <f t="shared" si="7"/>
@@ -40261,15 +40304,15 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P69" s="15">
+      <c r="P69" s="15" t="e">
         <f t="shared" si="13"/>
-        <v>52458</v>
+        <v>#REF!</v>
       </c>
       <c r="R69">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="S69">
-        <v>94.4</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.4">
@@ -40283,7 +40326,7 @@
         <v>434</v>
       </c>
       <c r="D70">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E70">
         <v>114</v>
@@ -40294,11 +40337,11 @@
       </c>
       <c r="G70">
         <f t="shared" si="10"/>
-        <v>422.79999999999995</v>
+        <v>428.08499999999998</v>
       </c>
       <c r="H70">
         <f t="shared" si="11"/>
-        <v>422.79999999999995</v>
+        <v>428.08499999999998</v>
       </c>
       <c r="I70">
         <f t="shared" si="12"/>
@@ -40315,12 +40358,12 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P70" s="15">
+      <c r="P70" s="15" t="e">
         <f t="shared" si="13"/>
-        <v>53256</v>
+        <v>#REF!</v>
       </c>
       <c r="R70">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="S70">
         <v>94.3</v>
@@ -40337,7 +40380,7 @@
         <v>434</v>
       </c>
       <c r="D71">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E71">
         <v>114</v>
@@ -40348,15 +40391,15 @@
       </c>
       <c r="G71">
         <f t="shared" si="10"/>
-        <v>428.08499999999998</v>
+        <v>433.78000000000003</v>
       </c>
       <c r="H71">
         <f t="shared" si="11"/>
-        <v>428.08499999999998</v>
+        <v>433.78000000000003</v>
       </c>
       <c r="I71">
         <f t="shared" si="12"/>
-        <v>5.7000000000000028</v>
+        <v>5.7999999999999972</v>
       </c>
       <c r="M71">
         <v>64.599999999999994</v>
@@ -40369,15 +40412,15 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P71" s="15">
+      <c r="P71" s="15" t="e">
         <f t="shared" si="13"/>
-        <v>54054</v>
+        <v>#REF!</v>
       </c>
       <c r="R71">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="S71">
-        <v>94.3</v>
+        <v>94.2</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.4">
@@ -40391,7 +40434,7 @@
         <v>434</v>
       </c>
       <c r="D72">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E72">
         <v>114</v>
@@ -40402,15 +40445,15 @@
       </c>
       <c r="G72">
         <f t="shared" si="10"/>
-        <v>433.78000000000003</v>
+        <v>439.48500000000007</v>
       </c>
       <c r="H72">
         <f t="shared" si="11"/>
-        <v>433.78000000000003</v>
+        <v>439.48500000000007</v>
       </c>
       <c r="I72">
         <f t="shared" si="12"/>
-        <v>5.7999999999999972</v>
+        <v>5.9000000000000057</v>
       </c>
       <c r="M72">
         <v>64.599999999999994</v>
@@ -40423,15 +40466,15 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P72" s="15">
+      <c r="P72" s="15" t="e">
         <f t="shared" si="13"/>
-        <v>54852</v>
+        <v>#REF!</v>
       </c>
       <c r="R72">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="S72">
-        <v>94.2</v>
+        <v>94.1</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.4">
@@ -40445,7 +40488,7 @@
         <v>434</v>
       </c>
       <c r="D73">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E73">
         <v>114</v>
@@ -40456,18 +40499,18 @@
       </c>
       <c r="G73">
         <f t="shared" si="10"/>
-        <v>439.48500000000007</v>
+        <v>445.20000000000005</v>
       </c>
       <c r="H73">
-        <f t="shared" si="11"/>
-        <v>439.48500000000007</v>
+        <f>G73</f>
+        <v>445.20000000000005</v>
       </c>
       <c r="I73">
         <f t="shared" si="12"/>
-        <v>5.9000000000000057</v>
+        <v>6</v>
       </c>
       <c r="M73">
-        <v>64.599999999999994</v>
+        <v>64.7</v>
       </c>
       <c r="N73" s="15">
         <f t="shared" si="7"/>
@@ -40477,279 +40520,65 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P73" s="15">
+      <c r="P73" s="15" t="e">
         <f t="shared" si="13"/>
-        <v>55650</v>
+        <v>#REF!</v>
       </c>
       <c r="R73">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="S73">
-        <v>94.1</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>537</v>
       </c>
-      <c r="B74" t="s">
-        <v>538</v>
-      </c>
-      <c r="C74" t="s">
-        <v>434</v>
-      </c>
-      <c r="D74">
-        <v>90</v>
-      </c>
-      <c r="E74">
-        <v>114</v>
-      </c>
-      <c r="F74">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
-      <c r="G74">
-        <f t="shared" si="10"/>
-        <v>445.20000000000005</v>
-      </c>
-      <c r="H74">
-        <f>G74</f>
-        <v>445.20000000000005</v>
-      </c>
-      <c r="I74">
-        <f t="shared" si="12"/>
-        <v>6</v>
-      </c>
-      <c r="M74">
-        <v>64.7</v>
-      </c>
-      <c r="N74" s="15">
-        <f t="shared" si="7"/>
-        <v>114</v>
-      </c>
-      <c r="O74" s="15">
-        <f t="shared" si="8"/>
-        <v>798</v>
-      </c>
-      <c r="P74" s="15">
-        <f t="shared" si="13"/>
-        <v>56448</v>
-      </c>
-      <c r="R74">
-        <v>420</v>
-      </c>
-      <c r="S74">
-        <v>94</v>
-      </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>537</v>
       </c>
-      <c r="B75" t="s">
-        <v>538</v>
-      </c>
-      <c r="C75" t="s">
-        <v>434</v>
-      </c>
-      <c r="D75">
-        <v>91</v>
-      </c>
-      <c r="E75">
-        <v>114</v>
-      </c>
-      <c r="F75">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>537</v>
       </c>
-      <c r="B76" t="s">
-        <v>538</v>
-      </c>
-      <c r="C76" t="s">
-        <v>434</v>
-      </c>
-      <c r="D76">
-        <v>92</v>
-      </c>
-      <c r="E76">
-        <v>114</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>537</v>
       </c>
-      <c r="B77" t="s">
-        <v>538</v>
-      </c>
-      <c r="C77" t="s">
-        <v>434</v>
-      </c>
-      <c r="D77">
-        <v>93</v>
-      </c>
-      <c r="E77">
-        <v>114</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>537</v>
       </c>
-      <c r="B78" t="s">
-        <v>538</v>
-      </c>
-      <c r="C78" t="s">
-        <v>434</v>
-      </c>
-      <c r="D78">
-        <v>94</v>
-      </c>
-      <c r="E78">
-        <v>114</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>537</v>
       </c>
-      <c r="B79" t="s">
-        <v>538</v>
-      </c>
-      <c r="C79" t="s">
-        <v>434</v>
-      </c>
-      <c r="D79">
-        <v>95</v>
-      </c>
-      <c r="E79">
-        <v>114</v>
-      </c>
-      <c r="F79">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>537</v>
       </c>
-      <c r="B80" t="s">
-        <v>538</v>
-      </c>
-      <c r="C80" t="s">
-        <v>434</v>
-      </c>
-      <c r="D80">
-        <v>96</v>
-      </c>
-      <c r="E80">
-        <v>114</v>
-      </c>
-      <c r="F80">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>537</v>
       </c>
-      <c r="B81" t="s">
-        <v>538</v>
-      </c>
-      <c r="C81" t="s">
-        <v>434</v>
-      </c>
-      <c r="D81">
-        <v>97</v>
-      </c>
-      <c r="E81">
-        <v>114</v>
-      </c>
-      <c r="F81">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>537</v>
       </c>
-      <c r="B82" t="s">
-        <v>538</v>
-      </c>
-      <c r="C82" t="s">
-        <v>434</v>
-      </c>
-      <c r="D82">
-        <v>98</v>
-      </c>
-      <c r="E82">
-        <v>114</v>
-      </c>
-      <c r="F82">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>537</v>
-      </c>
-      <c r="B83" t="s">
-        <v>538</v>
-      </c>
-      <c r="C83" t="s">
-        <v>434</v>
-      </c>
-      <c r="D83">
-        <v>99</v>
-      </c>
-      <c r="E83">
-        <v>114</v>
-      </c>
-      <c r="F83">
-        <f t="shared" si="9"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A84" t="s">
-        <v>537</v>
-      </c>
-      <c r="B84" t="s">
-        <v>538</v>
-      </c>
-      <c r="C84" t="s">
-        <v>434</v>
-      </c>
-      <c r="D84">
-        <v>100</v>
-      </c>
-      <c r="E84">
-        <v>114</v>
-      </c>
-      <c r="F84">
-        <f t="shared" si="9"/>
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -40758,9 +40587,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40987,27 +40819,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F100BD1-711E-496E-80A4-2273FC6E7D53}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5967F658-4267-4B6D-95A6-954A8A84F3DB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b3c8f6b3-6c85-4471-847b-a0aae48a3f18"/>
-    <ds:schemaRef ds:uri="4a34b3b2-3a15-4120-8339-8dd1846f4033"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -41032,9 +40852,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5967F658-4267-4B6D-95A6-954A8A84F3DB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F100BD1-711E-496E-80A4-2273FC6E7D53}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b3c8f6b3-6c85-4471-847b-a0aae48a3f18"/>
+    <ds:schemaRef ds:uri="4a34b3b2-3a15-4120-8339-8dd1846f4033"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
excel file adjust & corrections
</commit_message>
<xml_diff>
--- a/layers_dta.xlsx
+++ b/layers_dta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\python\layers performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1841202C-B6F5-4396-9D76-3D3C9800BE9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77336C1-D428-469F-8193-FA33C51E7E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2569" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2569" uniqueCount="459">
   <si>
     <r>
       <rPr>
@@ -4126,252 +4126,6 @@
   </si>
   <si>
     <t>egg_weight_avg</t>
-  </si>
-  <si>
-    <t>hyline_w37</t>
-  </si>
-  <si>
-    <t>hyline_w38</t>
-  </si>
-  <si>
-    <t>hyline_w39</t>
-  </si>
-  <si>
-    <t>hyline_w40</t>
-  </si>
-  <si>
-    <t>hyline_w41</t>
-  </si>
-  <si>
-    <t>hyline_w42</t>
-  </si>
-  <si>
-    <t>hyline_w43</t>
-  </si>
-  <si>
-    <t>hyline_w44</t>
-  </si>
-  <si>
-    <t>hyline_w45</t>
-  </si>
-  <si>
-    <t>hyline_w46</t>
-  </si>
-  <si>
-    <t>hyline_w47</t>
-  </si>
-  <si>
-    <t>hyline_w48</t>
-  </si>
-  <si>
-    <t>hyline_w49</t>
-  </si>
-  <si>
-    <t>hyline_w50</t>
-  </si>
-  <si>
-    <t>hyline_w51</t>
-  </si>
-  <si>
-    <t>hyline_w52</t>
-  </si>
-  <si>
-    <t>hyline_w53</t>
-  </si>
-  <si>
-    <t>hyline_w54</t>
-  </si>
-  <si>
-    <t>hyline_w55</t>
-  </si>
-  <si>
-    <t>hyline_w56</t>
-  </si>
-  <si>
-    <t>hyline_w57</t>
-  </si>
-  <si>
-    <t>hyline_w58</t>
-  </si>
-  <si>
-    <t>hyline_w59</t>
-  </si>
-  <si>
-    <t>hyline_w60</t>
-  </si>
-  <si>
-    <t>hyline_w61</t>
-  </si>
-  <si>
-    <t>hyline_w62</t>
-  </si>
-  <si>
-    <t>hyline_w63</t>
-  </si>
-  <si>
-    <t>hyline_w64</t>
-  </si>
-  <si>
-    <t>hyline_w65</t>
-  </si>
-  <si>
-    <t>hyline_w66</t>
-  </si>
-  <si>
-    <t>hyline_w67</t>
-  </si>
-  <si>
-    <t>hyline_w68</t>
-  </si>
-  <si>
-    <t>hyline_w69</t>
-  </si>
-  <si>
-    <t>hyline_w70</t>
-  </si>
-  <si>
-    <t>hyline_w71</t>
-  </si>
-  <si>
-    <t>hyline_w72</t>
-  </si>
-  <si>
-    <t>hyline_w73</t>
-  </si>
-  <si>
-    <t>hyline_w74</t>
-  </si>
-  <si>
-    <t>hyline_w75</t>
-  </si>
-  <si>
-    <t>hyline_w76</t>
-  </si>
-  <si>
-    <t>hyline_w77</t>
-  </si>
-  <si>
-    <t>hyline_w78</t>
-  </si>
-  <si>
-    <t>hyline_w79</t>
-  </si>
-  <si>
-    <t>hyline_w80</t>
-  </si>
-  <si>
-    <t>hyline_w81</t>
-  </si>
-  <si>
-    <t>hyline_w82</t>
-  </si>
-  <si>
-    <t>hyline_w83</t>
-  </si>
-  <si>
-    <t>hyline_w84</t>
-  </si>
-  <si>
-    <t>hyline_w85</t>
-  </si>
-  <si>
-    <t>hyline_w86</t>
-  </si>
-  <si>
-    <t>hyline_w87</t>
-  </si>
-  <si>
-    <t>hyline_w88</t>
-  </si>
-  <si>
-    <t>hyline_w89</t>
-  </si>
-  <si>
-    <t>hyline_w90</t>
-  </si>
-  <si>
-    <t>hyline_w91</t>
-  </si>
-  <si>
-    <t>hyline_w92</t>
-  </si>
-  <si>
-    <t>hyline_w93</t>
-  </si>
-  <si>
-    <t>hyline_w94</t>
-  </si>
-  <si>
-    <t>hyline_w95</t>
-  </si>
-  <si>
-    <t>hyline_w96</t>
-  </si>
-  <si>
-    <t>hyline_w97</t>
-  </si>
-  <si>
-    <t>hyline_w98</t>
-  </si>
-  <si>
-    <t>hyline_w99</t>
-  </si>
-  <si>
-    <t>hyline_w100</t>
-  </si>
-  <si>
-    <t>hyline_w101</t>
-  </si>
-  <si>
-    <t>hyline_w102</t>
-  </si>
-  <si>
-    <t>hyline_w103</t>
-  </si>
-  <si>
-    <t>hyline_w104</t>
-  </si>
-  <si>
-    <t>hyline_w105</t>
-  </si>
-  <si>
-    <t>hyline_w106</t>
-  </si>
-  <si>
-    <t>hyline_w107</t>
-  </si>
-  <si>
-    <t>hyline_w108</t>
-  </si>
-  <si>
-    <t>hyline_w109</t>
-  </si>
-  <si>
-    <t>hyline_w110</t>
-  </si>
-  <si>
-    <t>hyline_w111</t>
-  </si>
-  <si>
-    <t>hyline_w112</t>
-  </si>
-  <si>
-    <t>hyline_w113</t>
-  </si>
-  <si>
-    <t>hyline_w114</t>
-  </si>
-  <si>
-    <t>hyline_w115</t>
-  </si>
-  <si>
-    <t>hyline_w116</t>
-  </si>
-  <si>
-    <t>hyline_w117</t>
-  </si>
-  <si>
-    <t>hyline_w118</t>
   </si>
   <si>
     <t>avg_feed_hen_day</t>
@@ -23060,7 +22814,7 @@
         <v>400</v>
       </c>
       <c r="O1" t="s">
-        <v>534</v>
+        <v>452</v>
       </c>
       <c r="P1" t="s">
         <v>431</v>
@@ -28566,8 +28320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EFC6FC-9C18-491D-9371-04A10A5E2B2E}">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -28610,10 +28364,10 @@
         <v>437</v>
       </c>
       <c r="G1" t="s">
-        <v>535</v>
+        <v>453</v>
       </c>
       <c r="H1" t="s">
-        <v>536</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
         <v>428</v>
@@ -28631,10 +28385,10 @@
         <v>449</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>532</v>
+        <v>450</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>533</v>
+        <v>451</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>439</v>
@@ -28698,7 +28452,7 @@
         <v>433</v>
       </c>
       <c r="B3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C3" t="s">
         <v>448</v>
@@ -28745,7 +28499,7 @@
         <v>433</v>
       </c>
       <c r="B4" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C4" t="s">
         <v>448</v>
@@ -28792,7 +28546,7 @@
         <v>433</v>
       </c>
       <c r="B5" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C5" t="s">
         <v>448</v>
@@ -28839,7 +28593,7 @@
         <v>433</v>
       </c>
       <c r="B6" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C6" t="s">
         <v>448</v>
@@ -28886,7 +28640,7 @@
         <v>433</v>
       </c>
       <c r="B7" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="C7" t="s">
         <v>448</v>
@@ -28933,7 +28687,7 @@
         <v>433</v>
       </c>
       <c r="B8" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C8" t="s">
         <v>448</v>
@@ -28980,7 +28734,7 @@
         <v>433</v>
       </c>
       <c r="B9" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="C9" t="s">
         <v>448</v>
@@ -29027,7 +28781,7 @@
         <v>433</v>
       </c>
       <c r="B10" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="C10" t="s">
         <v>448</v>
@@ -29074,7 +28828,7 @@
         <v>433</v>
       </c>
       <c r="B11" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="C11" t="s">
         <v>448</v>
@@ -29121,7 +28875,7 @@
         <v>433</v>
       </c>
       <c r="B12" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="C12" t="s">
         <v>448</v>
@@ -29168,7 +28922,7 @@
         <v>433</v>
       </c>
       <c r="B13" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="C13" t="s">
         <v>448</v>
@@ -29215,7 +28969,7 @@
         <v>433</v>
       </c>
       <c r="B14" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="C14" t="s">
         <v>448</v>
@@ -29262,7 +29016,7 @@
         <v>433</v>
       </c>
       <c r="B15" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="C15" t="s">
         <v>448</v>
@@ -29309,7 +29063,7 @@
         <v>433</v>
       </c>
       <c r="B16" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="C16" t="s">
         <v>448</v>
@@ -29356,7 +29110,7 @@
         <v>433</v>
       </c>
       <c r="B17" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="C17" t="s">
         <v>448</v>
@@ -29403,7 +29157,7 @@
         <v>433</v>
       </c>
       <c r="B18" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="C18" t="s">
         <v>448</v>
@@ -29450,7 +29204,7 @@
         <v>433</v>
       </c>
       <c r="B19" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="C19" t="s">
         <v>448</v>
@@ -29497,7 +29251,7 @@
         <v>433</v>
       </c>
       <c r="B20" t="s">
-        <v>467</v>
+        <v>447</v>
       </c>
       <c r="C20" t="s">
         <v>448</v>
@@ -29544,7 +29298,7 @@
         <v>433</v>
       </c>
       <c r="B21" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="C21" t="s">
         <v>448</v>
@@ -29591,7 +29345,7 @@
         <v>433</v>
       </c>
       <c r="B22" t="s">
-        <v>469</v>
+        <v>447</v>
       </c>
       <c r="C22" t="s">
         <v>448</v>
@@ -29638,7 +29392,7 @@
         <v>433</v>
       </c>
       <c r="B23" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
       <c r="C23" t="s">
         <v>448</v>
@@ -29685,7 +29439,7 @@
         <v>433</v>
       </c>
       <c r="B24" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="C24" t="s">
         <v>448</v>
@@ -29732,7 +29486,7 @@
         <v>433</v>
       </c>
       <c r="B25" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="C25" t="s">
         <v>448</v>
@@ -29779,7 +29533,7 @@
         <v>433</v>
       </c>
       <c r="B26" t="s">
-        <v>473</v>
+        <v>447</v>
       </c>
       <c r="C26" t="s">
         <v>448</v>
@@ -29826,7 +29580,7 @@
         <v>433</v>
       </c>
       <c r="B27" t="s">
-        <v>474</v>
+        <v>447</v>
       </c>
       <c r="C27" t="s">
         <v>448</v>
@@ -29873,7 +29627,7 @@
         <v>433</v>
       </c>
       <c r="B28" t="s">
-        <v>475</v>
+        <v>447</v>
       </c>
       <c r="C28" t="s">
         <v>448</v>
@@ -29920,7 +29674,7 @@
         <v>433</v>
       </c>
       <c r="B29" t="s">
-        <v>476</v>
+        <v>447</v>
       </c>
       <c r="C29" t="s">
         <v>448</v>
@@ -29967,7 +29721,7 @@
         <v>433</v>
       </c>
       <c r="B30" t="s">
-        <v>477</v>
+        <v>447</v>
       </c>
       <c r="C30" t="s">
         <v>448</v>
@@ -30014,7 +29768,7 @@
         <v>433</v>
       </c>
       <c r="B31" t="s">
-        <v>478</v>
+        <v>447</v>
       </c>
       <c r="C31" t="s">
         <v>448</v>
@@ -30061,7 +29815,7 @@
         <v>433</v>
       </c>
       <c r="B32" t="s">
-        <v>479</v>
+        <v>447</v>
       </c>
       <c r="C32" t="s">
         <v>448</v>
@@ -30108,7 +29862,7 @@
         <v>433</v>
       </c>
       <c r="B33" t="s">
-        <v>480</v>
+        <v>447</v>
       </c>
       <c r="C33" t="s">
         <v>448</v>
@@ -30155,7 +29909,7 @@
         <v>433</v>
       </c>
       <c r="B34" t="s">
-        <v>481</v>
+        <v>447</v>
       </c>
       <c r="C34" t="s">
         <v>448</v>
@@ -30202,7 +29956,7 @@
         <v>433</v>
       </c>
       <c r="B35" t="s">
-        <v>482</v>
+        <v>447</v>
       </c>
       <c r="C35" t="s">
         <v>448</v>
@@ -30249,7 +30003,7 @@
         <v>433</v>
       </c>
       <c r="B36" t="s">
-        <v>483</v>
+        <v>447</v>
       </c>
       <c r="C36" t="s">
         <v>448</v>
@@ -30296,7 +30050,7 @@
         <v>433</v>
       </c>
       <c r="B37" t="s">
-        <v>484</v>
+        <v>447</v>
       </c>
       <c r="C37" t="s">
         <v>448</v>
@@ -30343,7 +30097,7 @@
         <v>433</v>
       </c>
       <c r="B38" t="s">
-        <v>485</v>
+        <v>447</v>
       </c>
       <c r="C38" t="s">
         <v>448</v>
@@ -30390,7 +30144,7 @@
         <v>433</v>
       </c>
       <c r="B39" t="s">
-        <v>486</v>
+        <v>447</v>
       </c>
       <c r="C39" t="s">
         <v>448</v>
@@ -30437,7 +30191,7 @@
         <v>433</v>
       </c>
       <c r="B40" t="s">
-        <v>487</v>
+        <v>447</v>
       </c>
       <c r="C40" t="s">
         <v>448</v>
@@ -30484,7 +30238,7 @@
         <v>433</v>
       </c>
       <c r="B41" t="s">
-        <v>488</v>
+        <v>447</v>
       </c>
       <c r="C41" t="s">
         <v>448</v>
@@ -30531,7 +30285,7 @@
         <v>433</v>
       </c>
       <c r="B42" t="s">
-        <v>489</v>
+        <v>447</v>
       </c>
       <c r="C42" t="s">
         <v>448</v>
@@ -30578,7 +30332,7 @@
         <v>433</v>
       </c>
       <c r="B43" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
       <c r="C43" t="s">
         <v>448</v>
@@ -30625,7 +30379,7 @@
         <v>433</v>
       </c>
       <c r="B44" t="s">
-        <v>491</v>
+        <v>447</v>
       </c>
       <c r="C44" t="s">
         <v>448</v>
@@ -30672,7 +30426,7 @@
         <v>433</v>
       </c>
       <c r="B45" t="s">
-        <v>492</v>
+        <v>447</v>
       </c>
       <c r="C45" t="s">
         <v>448</v>
@@ -30719,7 +30473,7 @@
         <v>433</v>
       </c>
       <c r="B46" t="s">
-        <v>493</v>
+        <v>447</v>
       </c>
       <c r="C46" t="s">
         <v>448</v>
@@ -30766,7 +30520,7 @@
         <v>433</v>
       </c>
       <c r="B47" t="s">
-        <v>494</v>
+        <v>447</v>
       </c>
       <c r="C47" t="s">
         <v>448</v>
@@ -30813,7 +30567,7 @@
         <v>433</v>
       </c>
       <c r="B48" t="s">
-        <v>495</v>
+        <v>447</v>
       </c>
       <c r="C48" t="s">
         <v>448</v>
@@ -30860,7 +30614,7 @@
         <v>433</v>
       </c>
       <c r="B49" t="s">
-        <v>496</v>
+        <v>447</v>
       </c>
       <c r="C49" t="s">
         <v>448</v>
@@ -30907,7 +30661,7 @@
         <v>433</v>
       </c>
       <c r="B50" t="s">
-        <v>497</v>
+        <v>447</v>
       </c>
       <c r="C50" t="s">
         <v>448</v>
@@ -30954,7 +30708,7 @@
         <v>433</v>
       </c>
       <c r="B51" t="s">
-        <v>498</v>
+        <v>447</v>
       </c>
       <c r="C51" t="s">
         <v>448</v>
@@ -31001,7 +30755,7 @@
         <v>433</v>
       </c>
       <c r="B52" t="s">
-        <v>499</v>
+        <v>447</v>
       </c>
       <c r="C52" t="s">
         <v>448</v>
@@ -31048,7 +30802,7 @@
         <v>433</v>
       </c>
       <c r="B53" t="s">
-        <v>500</v>
+        <v>447</v>
       </c>
       <c r="C53" t="s">
         <v>448</v>
@@ -31095,7 +30849,7 @@
         <v>433</v>
       </c>
       <c r="B54" t="s">
-        <v>501</v>
+        <v>447</v>
       </c>
       <c r="C54" t="s">
         <v>448</v>
@@ -31142,7 +30896,7 @@
         <v>433</v>
       </c>
       <c r="B55" t="s">
-        <v>502</v>
+        <v>447</v>
       </c>
       <c r="C55" t="s">
         <v>448</v>
@@ -31189,7 +30943,7 @@
         <v>433</v>
       </c>
       <c r="B56" t="s">
-        <v>503</v>
+        <v>447</v>
       </c>
       <c r="C56" t="s">
         <v>448</v>
@@ -31236,7 +30990,7 @@
         <v>433</v>
       </c>
       <c r="B57" t="s">
-        <v>504</v>
+        <v>447</v>
       </c>
       <c r="C57" t="s">
         <v>448</v>
@@ -31283,7 +31037,7 @@
         <v>433</v>
       </c>
       <c r="B58" t="s">
-        <v>505</v>
+        <v>447</v>
       </c>
       <c r="C58" t="s">
         <v>448</v>
@@ -31330,7 +31084,7 @@
         <v>433</v>
       </c>
       <c r="B59" t="s">
-        <v>506</v>
+        <v>447</v>
       </c>
       <c r="C59" t="s">
         <v>448</v>
@@ -31377,7 +31131,7 @@
         <v>433</v>
       </c>
       <c r="B60" t="s">
-        <v>507</v>
+        <v>447</v>
       </c>
       <c r="C60" t="s">
         <v>448</v>
@@ -31424,7 +31178,7 @@
         <v>433</v>
       </c>
       <c r="B61" t="s">
-        <v>508</v>
+        <v>447</v>
       </c>
       <c r="C61" t="s">
         <v>448</v>
@@ -31471,7 +31225,7 @@
         <v>433</v>
       </c>
       <c r="B62" t="s">
-        <v>509</v>
+        <v>447</v>
       </c>
       <c r="C62" t="s">
         <v>448</v>
@@ -31518,7 +31272,7 @@
         <v>433</v>
       </c>
       <c r="B63" t="s">
-        <v>510</v>
+        <v>447</v>
       </c>
       <c r="C63" t="s">
         <v>448</v>
@@ -31565,7 +31319,7 @@
         <v>433</v>
       </c>
       <c r="B64" t="s">
-        <v>511</v>
+        <v>447</v>
       </c>
       <c r="C64" t="s">
         <v>448</v>
@@ -31612,7 +31366,7 @@
         <v>433</v>
       </c>
       <c r="B65" t="s">
-        <v>512</v>
+        <v>447</v>
       </c>
       <c r="C65" t="s">
         <v>448</v>
@@ -31659,7 +31413,7 @@
         <v>433</v>
       </c>
       <c r="B66" t="s">
-        <v>513</v>
+        <v>447</v>
       </c>
       <c r="C66" t="s">
         <v>448</v>
@@ -31706,7 +31460,7 @@
         <v>433</v>
       </c>
       <c r="B67" t="s">
-        <v>514</v>
+        <v>447</v>
       </c>
       <c r="C67" t="s">
         <v>448</v>
@@ -31753,7 +31507,7 @@
         <v>433</v>
       </c>
       <c r="B68" t="s">
-        <v>515</v>
+        <v>447</v>
       </c>
       <c r="C68" t="s">
         <v>448</v>
@@ -31800,7 +31554,7 @@
         <v>433</v>
       </c>
       <c r="B69" t="s">
-        <v>516</v>
+        <v>447</v>
       </c>
       <c r="C69" t="s">
         <v>448</v>
@@ -31847,7 +31601,7 @@
         <v>433</v>
       </c>
       <c r="B70" t="s">
-        <v>517</v>
+        <v>447</v>
       </c>
       <c r="C70" t="s">
         <v>448</v>
@@ -31894,7 +31648,7 @@
         <v>433</v>
       </c>
       <c r="B71" t="s">
-        <v>518</v>
+        <v>447</v>
       </c>
       <c r="C71" t="s">
         <v>448</v>
@@ -31941,7 +31695,7 @@
         <v>433</v>
       </c>
       <c r="B72" t="s">
-        <v>519</v>
+        <v>447</v>
       </c>
       <c r="C72" t="s">
         <v>448</v>
@@ -31988,7 +31742,7 @@
         <v>433</v>
       </c>
       <c r="B73" t="s">
-        <v>520</v>
+        <v>447</v>
       </c>
       <c r="C73" t="s">
         <v>448</v>
@@ -32035,7 +31789,7 @@
         <v>433</v>
       </c>
       <c r="B74" t="s">
-        <v>521</v>
+        <v>447</v>
       </c>
       <c r="C74" t="s">
         <v>448</v>
@@ -32082,7 +31836,7 @@
         <v>433</v>
       </c>
       <c r="B75" t="s">
-        <v>522</v>
+        <v>447</v>
       </c>
       <c r="C75" t="s">
         <v>448</v>
@@ -32129,7 +31883,7 @@
         <v>433</v>
       </c>
       <c r="B76" t="s">
-        <v>523</v>
+        <v>447</v>
       </c>
       <c r="C76" t="s">
         <v>448</v>
@@ -32176,7 +31930,7 @@
         <v>433</v>
       </c>
       <c r="B77" t="s">
-        <v>524</v>
+        <v>447</v>
       </c>
       <c r="C77" t="s">
         <v>448</v>
@@ -32223,7 +31977,7 @@
         <v>433</v>
       </c>
       <c r="B78" t="s">
-        <v>525</v>
+        <v>447</v>
       </c>
       <c r="C78" t="s">
         <v>448</v>
@@ -32270,7 +32024,7 @@
         <v>433</v>
       </c>
       <c r="B79" t="s">
-        <v>526</v>
+        <v>447</v>
       </c>
       <c r="C79" t="s">
         <v>448</v>
@@ -32317,7 +32071,7 @@
         <v>433</v>
       </c>
       <c r="B80" t="s">
-        <v>527</v>
+        <v>447</v>
       </c>
       <c r="C80" t="s">
         <v>448</v>
@@ -32364,7 +32118,7 @@
         <v>433</v>
       </c>
       <c r="B81" t="s">
-        <v>528</v>
+        <v>447</v>
       </c>
       <c r="C81" t="s">
         <v>448</v>
@@ -32411,7 +32165,7 @@
         <v>433</v>
       </c>
       <c r="B82" t="s">
-        <v>529</v>
+        <v>447</v>
       </c>
       <c r="C82" t="s">
         <v>448</v>
@@ -32458,7 +32212,7 @@
         <v>433</v>
       </c>
       <c r="B83" t="s">
-        <v>530</v>
+        <v>447</v>
       </c>
       <c r="C83" t="s">
         <v>448</v>
@@ -32505,7 +32259,7 @@
         <v>433</v>
       </c>
       <c r="B84" t="s">
-        <v>531</v>
+        <v>447</v>
       </c>
       <c r="C84" t="s">
         <v>448</v>
@@ -32601,10 +32355,10 @@
         <v>437</v>
       </c>
       <c r="G1" t="s">
-        <v>535</v>
+        <v>453</v>
       </c>
       <c r="H1" t="s">
-        <v>536</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
         <v>428</v>
@@ -32622,10 +32376,10 @@
         <v>449</v>
       </c>
       <c r="N1" t="s">
-        <v>532</v>
+        <v>450</v>
       </c>
       <c r="O1" t="s">
-        <v>533</v>
+        <v>451</v>
       </c>
       <c r="P1" t="s">
         <v>439</v>
@@ -36563,20 +36317,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E3787F-904D-4FED-BBDE-8BED3DDF4D86}">
   <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="13.61328125" customWidth="1"/>
-    <col min="2" max="2" width="13.07421875" customWidth="1"/>
-    <col min="3" max="3" width="13.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" customWidth="1"/>
+    <col min="3" max="3" width="11.3828125" customWidth="1"/>
     <col min="4" max="4" width="16.61328125" customWidth="1"/>
     <col min="5" max="5" width="16.3828125" customWidth="1"/>
     <col min="6" max="6" width="17.07421875" customWidth="1"/>
     <col min="7" max="7" width="21.15234375" customWidth="1"/>
-    <col min="8" max="8" width="18.15234375" customWidth="1"/>
+    <col min="8" max="8" width="21.69140625" customWidth="1"/>
     <col min="9" max="9" width="22.53515625" customWidth="1"/>
     <col min="10" max="10" width="18.61328125" customWidth="1"/>
     <col min="11" max="11" width="14.15234375" customWidth="1"/>
@@ -36607,10 +36361,10 @@
         <v>437</v>
       </c>
       <c r="G1" t="s">
-        <v>535</v>
+        <v>453</v>
       </c>
       <c r="H1" t="s">
-        <v>536</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
         <v>428</v>
@@ -36628,27 +36382,27 @@
         <v>449</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>532</v>
+        <v>450</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>533</v>
+        <v>451</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>439</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>539</v>
+        <v>457</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>540</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B2" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C2" t="s">
         <v>434</v>
@@ -36686,9 +36440,9 @@
         <f t="shared" ref="O2:O65" si="1">N2*7</f>
         <v>623</v>
       </c>
-      <c r="P2" s="15" t="e">
-        <f>#REF!+O2</f>
-        <v>#REF!</v>
+      <c r="P2" s="15">
+        <f>O2</f>
+        <v>623</v>
       </c>
       <c r="R2">
         <v>1</v>
@@ -36699,10 +36453,10 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B3" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C3" t="s">
         <v>434</v>
@@ -36740,9 +36494,9 @@
         <f t="shared" si="1"/>
         <v>679</v>
       </c>
-      <c r="P3" s="15" t="e">
+      <c r="P3" s="15">
         <f t="shared" ref="P3:P66" si="6">P2+O3</f>
-        <v>#REF!</v>
+        <v>1302</v>
       </c>
       <c r="R3">
         <v>4</v>
@@ -36753,10 +36507,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B4" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C4" t="s">
         <v>434</v>
@@ -36794,9 +36548,9 @@
         <f t="shared" si="1"/>
         <v>728</v>
       </c>
-      <c r="P4" s="15" t="e">
+      <c r="P4" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>2030</v>
       </c>
       <c r="R4">
         <v>9</v>
@@ -36807,10 +36561,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B5" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C5" t="s">
         <v>434</v>
@@ -36848,9 +36602,9 @@
         <f t="shared" si="1"/>
         <v>770</v>
       </c>
-      <c r="P5" s="15" t="e">
+      <c r="P5" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>2800</v>
       </c>
       <c r="R5">
         <v>14</v>
@@ -36861,10 +36615,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B6" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C6" t="s">
         <v>434</v>
@@ -36902,9 +36656,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P6" s="15" t="e">
+      <c r="P6" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>3584</v>
       </c>
       <c r="R6">
         <v>21</v>
@@ -36915,10 +36669,10 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B7" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C7" t="s">
         <v>434</v>
@@ -36956,9 +36710,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P7" s="15" t="e">
+      <c r="P7" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>4368</v>
       </c>
       <c r="R7">
         <v>28</v>
@@ -36969,10 +36723,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B8" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C8" t="s">
         <v>434</v>
@@ -37010,9 +36764,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P8" s="15" t="e">
+      <c r="P8" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>5152</v>
       </c>
       <c r="R8">
         <v>34</v>
@@ -37023,10 +36777,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B9" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C9" t="s">
         <v>434</v>
@@ -37064,9 +36818,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P9" s="15" t="e">
+      <c r="P9" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>5936</v>
       </c>
       <c r="R9">
         <v>41</v>
@@ -37077,10 +36831,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B10" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C10" t="s">
         <v>434</v>
@@ -37118,9 +36872,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P10" s="15" t="e">
+      <c r="P10" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>6720</v>
       </c>
       <c r="R10">
         <v>48</v>
@@ -37131,10 +36885,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B11" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C11" t="s">
         <v>434</v>
@@ -37172,9 +36926,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P11" s="15" t="e">
+      <c r="P11" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>7504</v>
       </c>
       <c r="R11">
         <v>54</v>
@@ -37185,10 +36939,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B12" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C12" t="s">
         <v>434</v>
@@ -37226,9 +36980,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P12" s="15" t="e">
+      <c r="P12" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>8288</v>
       </c>
       <c r="R12">
         <v>61</v>
@@ -37239,10 +36993,10 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B13" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C13" t="s">
         <v>434</v>
@@ -37280,9 +37034,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P13" s="15" t="e">
+      <c r="P13" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>9072</v>
       </c>
       <c r="R13">
         <v>68</v>
@@ -37293,10 +37047,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B14" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C14" t="s">
         <v>434</v>
@@ -37334,9 +37088,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P14" s="15" t="e">
+      <c r="P14" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>9856</v>
       </c>
       <c r="R14">
         <v>74</v>
@@ -37347,10 +37101,10 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B15" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C15" t="s">
         <v>434</v>
@@ -37388,9 +37142,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P15" s="15" t="e">
+      <c r="P15" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>10640</v>
       </c>
       <c r="R15">
         <v>81</v>
@@ -37401,10 +37155,10 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B16" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C16" t="s">
         <v>434</v>
@@ -37442,9 +37196,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P16" s="15" t="e">
+      <c r="P16" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>11424</v>
       </c>
       <c r="R16">
         <v>87</v>
@@ -37455,10 +37209,10 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B17" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C17" t="s">
         <v>434</v>
@@ -37496,9 +37250,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P17" s="15" t="e">
+      <c r="P17" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>12208</v>
       </c>
       <c r="R17">
         <v>94</v>
@@ -37509,10 +37263,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B18" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C18" t="s">
         <v>434</v>
@@ -37550,9 +37304,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P18" s="15" t="e">
+      <c r="P18" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>12992</v>
       </c>
       <c r="R18">
         <v>101</v>
@@ -37563,10 +37317,10 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B19" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C19" t="s">
         <v>434</v>
@@ -37604,9 +37358,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P19" s="15" t="e">
+      <c r="P19" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>13776</v>
       </c>
       <c r="R19">
         <v>107</v>
@@ -37617,10 +37371,10 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B20" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C20" t="s">
         <v>434</v>
@@ -37658,9 +37412,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P20" s="15" t="e">
+      <c r="P20" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>14560</v>
       </c>
       <c r="R20">
         <v>114</v>
@@ -37671,10 +37425,10 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B21" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C21" t="s">
         <v>434</v>
@@ -37712,9 +37466,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P21" s="15" t="e">
+      <c r="P21" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>15344</v>
       </c>
       <c r="R21">
         <v>120</v>
@@ -37725,10 +37479,10 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B22" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C22" t="s">
         <v>434</v>
@@ -37766,9 +37520,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P22" s="15" t="e">
+      <c r="P22" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>16128</v>
       </c>
       <c r="R22">
         <v>127</v>
@@ -37779,10 +37533,10 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B23" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C23" t="s">
         <v>434</v>
@@ -37820,9 +37574,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P23" s="15" t="e">
+      <c r="P23" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>16912</v>
       </c>
       <c r="R23">
         <v>133</v>
@@ -37833,10 +37587,10 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B24" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C24" t="s">
         <v>434</v>
@@ -37874,9 +37628,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P24" s="15" t="e">
+      <c r="P24" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>17696</v>
       </c>
       <c r="R24">
         <v>140</v>
@@ -37887,10 +37641,10 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B25" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C25" t="s">
         <v>434</v>
@@ -37928,9 +37682,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P25" s="15" t="e">
+      <c r="P25" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>18480</v>
       </c>
       <c r="R25">
         <v>146</v>
@@ -37941,10 +37695,10 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B26" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C26" t="s">
         <v>434</v>
@@ -37982,9 +37736,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P26" s="15" t="e">
+      <c r="P26" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>19264</v>
       </c>
       <c r="R26">
         <v>153</v>
@@ -37995,10 +37749,10 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B27" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C27" t="s">
         <v>434</v>
@@ -38036,9 +37790,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P27" s="15" t="e">
+      <c r="P27" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>20048</v>
       </c>
       <c r="R27">
         <v>159</v>
@@ -38049,10 +37803,10 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B28" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C28" t="s">
         <v>434</v>
@@ -38090,9 +37844,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P28" s="15" t="e">
+      <c r="P28" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>20832</v>
       </c>
       <c r="R28">
         <v>165</v>
@@ -38103,10 +37857,10 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B29" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C29" t="s">
         <v>434</v>
@@ -38144,9 +37898,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P29" s="15" t="e">
+      <c r="P29" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>21616</v>
       </c>
       <c r="R29">
         <v>172</v>
@@ -38157,10 +37911,10 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B30" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C30" t="s">
         <v>434</v>
@@ -38198,9 +37952,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P30" s="15" t="e">
+      <c r="P30" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>22400</v>
       </c>
       <c r="R30">
         <v>178</v>
@@ -38211,10 +37965,10 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B31" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C31" t="s">
         <v>434</v>
@@ -38252,9 +38006,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P31" s="15" t="e">
+      <c r="P31" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>23184</v>
       </c>
       <c r="R31">
         <v>184</v>
@@ -38265,10 +38019,10 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B32" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C32" t="s">
         <v>434</v>
@@ -38306,9 +38060,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P32" s="15" t="e">
+      <c r="P32" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>23968</v>
       </c>
       <c r="R32">
         <v>191</v>
@@ -38319,10 +38073,10 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B33" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C33" t="s">
         <v>434</v>
@@ -38360,9 +38114,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P33" s="15" t="e">
+      <c r="P33" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>24752</v>
       </c>
       <c r="R33">
         <v>197</v>
@@ -38373,10 +38127,10 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B34" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C34" t="s">
         <v>434</v>
@@ -38414,9 +38168,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P34" s="15" t="e">
+      <c r="P34" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>25536</v>
       </c>
       <c r="R34">
         <v>203</v>
@@ -38427,10 +38181,10 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B35" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C35" t="s">
         <v>434</v>
@@ -38468,9 +38222,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P35" s="15" t="e">
+      <c r="P35" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>26320</v>
       </c>
       <c r="R35">
         <v>209</v>
@@ -38481,10 +38235,10 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B36" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C36" t="s">
         <v>434</v>
@@ -38522,9 +38276,9 @@
         <f t="shared" si="1"/>
         <v>784</v>
       </c>
-      <c r="P36" s="15" t="e">
+      <c r="P36" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>27104</v>
       </c>
       <c r="R36">
         <v>216</v>
@@ -38535,10 +38289,10 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B37" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C37" t="s">
         <v>434</v>
@@ -38576,9 +38330,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P37" s="15" t="e">
+      <c r="P37" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>27895</v>
       </c>
       <c r="R37">
         <v>222</v>
@@ -38589,10 +38343,10 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B38" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C38" t="s">
         <v>434</v>
@@ -38630,9 +38384,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P38" s="15" t="e">
+      <c r="P38" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>28686</v>
       </c>
       <c r="R38">
         <v>228</v>
@@ -38643,10 +38397,10 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B39" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C39" t="s">
         <v>434</v>
@@ -38684,9 +38438,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P39" s="15" t="e">
+      <c r="P39" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>29477</v>
       </c>
       <c r="R39">
         <v>234</v>
@@ -38697,10 +38451,10 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B40" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C40" t="s">
         <v>434</v>
@@ -38738,9 +38492,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P40" s="15" t="e">
+      <c r="P40" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>30268</v>
       </c>
       <c r="R40">
         <v>240</v>
@@ -38751,10 +38505,10 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B41" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C41" t="s">
         <v>434</v>
@@ -38792,9 +38546,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P41" s="15" t="e">
+      <c r="P41" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>31059</v>
       </c>
       <c r="R41">
         <v>246</v>
@@ -38805,10 +38559,10 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B42" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C42" t="s">
         <v>434</v>
@@ -38846,9 +38600,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P42" s="15" t="e">
+      <c r="P42" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>31850</v>
       </c>
       <c r="R42">
         <v>252</v>
@@ -38859,10 +38613,10 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B43" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C43" t="s">
         <v>434</v>
@@ -38900,9 +38654,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P43" s="15" t="e">
+      <c r="P43" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>32641</v>
       </c>
       <c r="R43">
         <v>258</v>
@@ -38913,10 +38667,10 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B44" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C44" t="s">
         <v>434</v>
@@ -38954,9 +38708,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P44" s="15" t="e">
+      <c r="P44" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>33432</v>
       </c>
       <c r="R44">
         <v>264</v>
@@ -38967,10 +38721,10 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B45" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C45" t="s">
         <v>434</v>
@@ -39008,9 +38762,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P45" s="15" t="e">
+      <c r="P45" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>34223</v>
       </c>
       <c r="R45">
         <v>270</v>
@@ -39021,10 +38775,10 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B46" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C46" t="s">
         <v>434</v>
@@ -39062,9 +38816,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P46" s="15" t="e">
+      <c r="P46" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>35014</v>
       </c>
       <c r="R46">
         <v>276</v>
@@ -39075,10 +38829,10 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B47" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C47" t="s">
         <v>434</v>
@@ -39116,9 +38870,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P47" s="15" t="e">
+      <c r="P47" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>35805</v>
       </c>
       <c r="R47">
         <v>281</v>
@@ -39129,10 +38883,10 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B48" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C48" t="s">
         <v>434</v>
@@ -39170,9 +38924,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P48" s="15" t="e">
+      <c r="P48" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>36596</v>
       </c>
       <c r="R48">
         <v>287</v>
@@ -39183,10 +38937,10 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B49" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C49" t="s">
         <v>434</v>
@@ -39224,9 +38978,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P49" s="15" t="e">
+      <c r="P49" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>37387</v>
       </c>
       <c r="R49">
         <v>293</v>
@@ -39237,10 +38991,10 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B50" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C50" t="s">
         <v>434</v>
@@ -39278,9 +39032,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P50" s="15" t="e">
+      <c r="P50" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>38178</v>
       </c>
       <c r="R50">
         <v>299</v>
@@ -39291,10 +39045,10 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B51" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C51" t="s">
         <v>434</v>
@@ -39332,9 +39086,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P51" s="15" t="e">
+      <c r="P51" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>38969</v>
       </c>
       <c r="R51">
         <v>304</v>
@@ -39345,10 +39099,10 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B52" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C52" t="s">
         <v>434</v>
@@ -39386,9 +39140,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P52" s="15" t="e">
+      <c r="P52" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>39760</v>
       </c>
       <c r="R52">
         <v>310</v>
@@ -39399,10 +39153,10 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B53" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C53" t="s">
         <v>434</v>
@@ -39440,9 +39194,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P53" s="15" t="e">
+      <c r="P53" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>40551</v>
       </c>
       <c r="R53">
         <v>315</v>
@@ -39453,10 +39207,10 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B54" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C54" t="s">
         <v>434</v>
@@ -39494,9 +39248,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P54" s="15" t="e">
+      <c r="P54" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>41342</v>
       </c>
       <c r="R54">
         <v>321</v>
@@ -39507,10 +39261,10 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B55" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C55" t="s">
         <v>434</v>
@@ -39548,9 +39302,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P55" s="15" t="e">
+      <c r="P55" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>42133</v>
       </c>
       <c r="R55">
         <v>327</v>
@@ -39561,10 +39315,10 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B56" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C56" t="s">
         <v>434</v>
@@ -39602,9 +39356,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P56" s="15" t="e">
+      <c r="P56" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>42924</v>
       </c>
       <c r="R56">
         <v>332</v>
@@ -39615,10 +39369,10 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B57" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C57" t="s">
         <v>434</v>
@@ -39656,9 +39410,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P57" s="15" t="e">
+      <c r="P57" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>43715</v>
       </c>
       <c r="R57">
         <v>337</v>
@@ -39669,10 +39423,10 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B58" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C58" t="s">
         <v>434</v>
@@ -39710,9 +39464,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P58" s="15" t="e">
+      <c r="P58" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>44506</v>
       </c>
       <c r="R58">
         <v>343</v>
@@ -39723,10 +39477,10 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B59" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C59" t="s">
         <v>434</v>
@@ -39764,9 +39518,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P59" s="15" t="e">
+      <c r="P59" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>45297</v>
       </c>
       <c r="R59">
         <v>348</v>
@@ -39777,10 +39531,10 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B60" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C60" t="s">
         <v>434</v>
@@ -39818,9 +39572,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P60" s="15" t="e">
+      <c r="P60" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>46088</v>
       </c>
       <c r="R60">
         <v>354</v>
@@ -39831,10 +39585,10 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B61" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C61" t="s">
         <v>434</v>
@@ -39872,9 +39626,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P61" s="15" t="e">
+      <c r="P61" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>46879</v>
       </c>
       <c r="R61">
         <v>359</v>
@@ -39885,10 +39639,10 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B62" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C62" t="s">
         <v>434</v>
@@ -39926,9 +39680,9 @@
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P62" s="15" t="e">
+      <c r="P62" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>47670</v>
       </c>
       <c r="R62">
         <v>364</v>
@@ -39939,10 +39693,10 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B63" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C63" t="s">
         <v>434</v>
@@ -39980,9 +39734,9 @@
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
-      <c r="P63" s="15" t="e">
+      <c r="P63" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>48468</v>
       </c>
       <c r="R63">
         <v>369</v>
@@ -39993,10 +39747,10 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B64" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C64" t="s">
         <v>434</v>
@@ -40034,9 +39788,9 @@
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
-      <c r="P64" s="15" t="e">
+      <c r="P64" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>49266</v>
       </c>
       <c r="R64">
         <v>375</v>
@@ -40047,10 +39801,10 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B65" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C65" t="s">
         <v>434</v>
@@ -40088,9 +39842,9 @@
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
-      <c r="P65" s="15" t="e">
+      <c r="P65" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>50064</v>
       </c>
       <c r="R65">
         <v>380</v>
@@ -40101,10 +39855,10 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B66" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C66" t="s">
         <v>434</v>
@@ -40142,9 +39896,9 @@
         <f t="shared" ref="O66:O73" si="8">N66*7</f>
         <v>798</v>
       </c>
-      <c r="P66" s="15" t="e">
+      <c r="P66" s="15">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
+        <v>50862</v>
       </c>
       <c r="R66">
         <v>385</v>
@@ -40155,10 +39909,10 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B67" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C67" t="s">
         <v>434</v>
@@ -40196,9 +39950,9 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P67" s="15" t="e">
+      <c r="P67" s="15">
         <f t="shared" ref="P67:P73" si="13">P66+O67</f>
-        <v>#REF!</v>
+        <v>51660</v>
       </c>
       <c r="R67">
         <v>390</v>
@@ -40209,10 +39963,10 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B68" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C68" t="s">
         <v>434</v>
@@ -40250,9 +40004,9 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P68" s="15" t="e">
+      <c r="P68" s="15">
         <f t="shared" si="13"/>
-        <v>#REF!</v>
+        <v>52458</v>
       </c>
       <c r="R68">
         <v>395</v>
@@ -40263,10 +40017,10 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B69" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C69" t="s">
         <v>434</v>
@@ -40304,9 +40058,9 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P69" s="15" t="e">
+      <c r="P69" s="15">
         <f t="shared" si="13"/>
-        <v>#REF!</v>
+        <v>53256</v>
       </c>
       <c r="R69">
         <v>400</v>
@@ -40317,10 +40071,10 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B70" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C70" t="s">
         <v>434</v>
@@ -40358,9 +40112,9 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P70" s="15" t="e">
+      <c r="P70" s="15">
         <f t="shared" si="13"/>
-        <v>#REF!</v>
+        <v>54054</v>
       </c>
       <c r="R70">
         <v>405</v>
@@ -40371,10 +40125,10 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B71" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C71" t="s">
         <v>434</v>
@@ -40412,9 +40166,9 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P71" s="15" t="e">
+      <c r="P71" s="15">
         <f t="shared" si="13"/>
-        <v>#REF!</v>
+        <v>54852</v>
       </c>
       <c r="R71">
         <v>410</v>
@@ -40425,10 +40179,10 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B72" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C72" t="s">
         <v>434</v>
@@ -40466,9 +40220,9 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P72" s="15" t="e">
+      <c r="P72" s="15">
         <f t="shared" si="13"/>
-        <v>#REF!</v>
+        <v>55650</v>
       </c>
       <c r="R72">
         <v>415</v>
@@ -40479,10 +40233,10 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="B73" t="s">
-        <v>538</v>
+        <v>456</v>
       </c>
       <c r="C73" t="s">
         <v>434</v>
@@ -40520,9 +40274,9 @@
         <f t="shared" si="8"/>
         <v>798</v>
       </c>
-      <c r="P73" s="15" t="e">
+      <c r="P73" s="15">
         <f t="shared" si="13"/>
-        <v>#REF!</v>
+        <v>56448</v>
       </c>
       <c r="R73">
         <v>420</v>
@@ -40533,52 +40287,52 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>